<commit_message>
correcting error in top20
</commit_message>
<xml_diff>
--- a/results/example/rate.xlsx
+++ b/results/example/rate.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
-  <si>
-    <t>P9</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+  <si>
+    <t>P9_ultra</t>
   </si>
   <si>
     <t>P9+BB_slnc</t>
@@ -31,6 +31,12 @@
     <t>BB_r</t>
   </si>
   <si>
+    <t>CIN-P9-1_l</t>
+  </si>
+  <si>
+    <t>CIN-P9-1_r</t>
+  </si>
+  <si>
     <t>DNa01_l</t>
   </si>
   <si>
@@ -67,24 +73,27 @@
     <t>MooDNg_l</t>
   </si>
   <si>
-    <t>P9-0DN1_l</t>
-  </si>
-  <si>
-    <t>P9-0DN1_r</t>
-  </si>
-  <si>
     <t>P9-cDN1_l</t>
   </si>
   <si>
     <t>P9-cDN1_r</t>
   </si>
   <si>
+    <t>P9-oDN1_l</t>
+  </si>
+  <si>
+    <t>P9-oDN1_r</t>
+  </si>
+  <si>
     <t>P9_l</t>
   </si>
   <si>
     <t>P9_r</t>
   </si>
   <si>
+    <t>neck motor neuron_r</t>
+  </si>
+  <si>
     <t>720575940604735660</t>
   </si>
   <si>
@@ -115,6 +124,9 @@
     <t>720575940606667868</t>
   </si>
   <si>
+    <t>720575940606852018</t>
+  </si>
+  <si>
     <t>720575940607641010</t>
   </si>
   <si>
@@ -145,7 +157,7 @@
     <t>720575940611206514</t>
   </si>
   <si>
-    <t>720575940612629210</t>
+    <t>720575940611772514</t>
   </si>
   <si>
     <t>720575940612766515</t>
@@ -163,6 +175,9 @@
     <t>720575940614963359</t>
   </si>
   <si>
+    <t>720575940615484063</t>
+  </si>
+  <si>
     <t>720575940615626562</t>
   </si>
   <si>
@@ -175,6 +190,9 @@
     <t>720575940615997919</t>
   </si>
   <si>
+    <t>720575940616018956</t>
+  </si>
+  <si>
     <t>720575940616566203</t>
   </si>
   <si>
@@ -214,7 +232,7 @@
     <t>720575940618156829</t>
   </si>
   <si>
-    <t>720575940618165393</t>
+    <t>720575940618167579</t>
   </si>
   <si>
     <t>720575940618177977</t>
@@ -241,6 +259,9 @@
     <t>720575940619681006</t>
   </si>
   <si>
+    <t>720575940619866027</t>
+  </si>
+  <si>
     <t>720575940619876884</t>
   </si>
   <si>
@@ -253,6 +274,9 @@
     <t>720575940620231590</t>
   </si>
   <si>
+    <t>720575940620250328</t>
+  </si>
+  <si>
     <t>720575940620282900</t>
   </si>
   <si>
@@ -313,9 +337,6 @@
     <t>720575940622933130</t>
   </si>
   <si>
-    <t>720575940622998627</t>
-  </si>
-  <si>
     <t>720575940623164515</t>
   </si>
   <si>
@@ -331,6 +352,9 @@
     <t>720575940624163303</t>
   </si>
   <si>
+    <t>720575940624231143</t>
+  </si>
+  <si>
     <t>720575940624336115</t>
   </si>
   <si>
@@ -370,6 +394,9 @@
     <t>720575940626210536</t>
   </si>
   <si>
+    <t>720575940626279486</t>
+  </si>
+  <si>
     <t>720575940626310960</t>
   </si>
   <si>
@@ -388,6 +415,9 @@
     <t>720575940626773523</t>
   </si>
   <si>
+    <t>720575940626812218</t>
+  </si>
+  <si>
     <t>720575940626829852</t>
   </si>
   <si>
@@ -403,6 +433,9 @@
     <t>720575940627348057</t>
   </si>
   <si>
+    <t>720575940627358853</t>
+  </si>
+  <si>
     <t>720575940627361157</t>
   </si>
   <si>
@@ -466,15 +499,18 @@
     <t>720575940630291767</t>
   </si>
   <si>
+    <t>720575940630808591</t>
+  </si>
+  <si>
     <t>720575940630931999</t>
   </si>
   <si>
+    <t>720575940631283267</t>
+  </si>
+  <si>
     <t>720575940631283512</t>
   </si>
   <si>
-    <t>720575940631715896</t>
-  </si>
-  <si>
     <t>720575940631721785</t>
   </si>
   <si>
@@ -505,12 +541,18 @@
     <t>720575940632943315</t>
   </si>
   <si>
+    <t>720575940632944339</t>
+  </si>
+  <si>
     <t>720575940632962786</t>
   </si>
   <si>
     <t>720575940633116256</t>
   </si>
   <si>
+    <t>720575940633270497</t>
+  </si>
+  <si>
     <t>720575940633308371</t>
   </si>
   <si>
@@ -529,12 +571,18 @@
     <t>720575940635170484</t>
   </si>
   <si>
+    <t>720575940635179359</t>
+  </si>
+  <si>
     <t>720575940635771316</t>
   </si>
   <si>
     <t>720575940635776760</t>
   </si>
   <si>
+    <t>720575940635937678</t>
+  </si>
+  <si>
     <t>720575940635942507</t>
   </si>
   <si>
@@ -544,6 +592,9 @@
     <t>720575940636879534</t>
   </si>
   <si>
+    <t>720575940636933751</t>
+  </si>
+  <si>
     <t>720575940637308605</t>
   </si>
   <si>
@@ -553,7 +604,10 @@
     <t>720575940638169917</t>
   </si>
   <si>
-    <t>720575940638664355</t>
+    <t>720575940638196038</t>
+  </si>
+  <si>
+    <t>720575940638681917</t>
   </si>
   <si>
     <t>720575940638989894</t>
@@ -571,6 +625,9 @@
     <t>720575940640696027</t>
   </si>
   <si>
+    <t>720575940641480949</t>
+  </si>
+  <si>
     <t>720575940641585627</t>
   </si>
   <si>
@@ -584,6 +641,9 @@
   </si>
   <si>
     <t>720575940644758308</t>
+  </si>
+  <si>
+    <t>720575940645047831</t>
   </si>
   <si>
     <t>720575940646126190</t>
@@ -975,7 +1035,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1008,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>109.7666666666667</v>
+        <v>109.5666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1019,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>111</v>
+        <v>113.6666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1027,10 +1087,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>28.16666666666667</v>
+        <v>13.9</v>
       </c>
       <c r="C4">
-        <v>16.33333333333333</v>
+        <v>3.714285714285714</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1038,10 +1098,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>19</v>
+        <v>21.66666666666667</v>
       </c>
       <c r="C5">
-        <v>12.2</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1049,10 +1109,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>27.43333333333333</v>
+        <v>42.63333333333333</v>
       </c>
       <c r="C6">
-        <v>15.4</v>
+        <v>15.86666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1060,10 +1120,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>10.53333333333333</v>
+        <v>34.13333333333333</v>
       </c>
       <c r="C7">
-        <v>5.8</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1071,10 +1131,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>29</v>
+        <v>37.76666666666667</v>
       </c>
       <c r="C8">
-        <v>18.6</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1082,10 +1142,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>22.83333333333333</v>
+        <v>16.3</v>
       </c>
       <c r="C9">
-        <v>12.4</v>
+        <v>5.366666666666666</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1093,10 +1153,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>11</v>
+        <v>29.53333333333333</v>
       </c>
       <c r="C10">
-        <v>6.133333333333334</v>
+        <v>17.76666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1104,10 +1164,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>8.233333333333333</v>
+        <v>26.66666666666667</v>
       </c>
       <c r="C11">
-        <v>4.466666666666667</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1115,10 +1175,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>17.16666666666667</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>6.166666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1126,10 +1186,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>1.333333333333333</v>
+        <v>16.8</v>
       </c>
       <c r="C13">
-        <v>1.421052631578947</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1137,10 +1197,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>2.931034482758621</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1148,10 +1208,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>5.6</v>
+        <v>13.8</v>
       </c>
       <c r="C15">
-        <v>2.133333333333333</v>
+        <v>1.578947368421053</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1159,10 +1219,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>20.73333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C16">
-        <v>9.800000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1170,10 +1230,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="1">
-        <v>25.9</v>
+        <v>10.53333333333333</v>
       </c>
       <c r="C17">
-        <v>12.36666666666667</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1181,10 +1241,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>22.4</v>
+        <v>27</v>
       </c>
       <c r="C18">
-        <v>10.66666666666667</v>
+        <v>10.36666666666667</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1192,10 +1252,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>13.8</v>
+        <v>13.16666666666667</v>
       </c>
       <c r="C19">
-        <v>6.5</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1203,10 +1263,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>151.9</v>
+        <v>35.26666666666667</v>
       </c>
       <c r="C20">
-        <v>149.2</v>
+        <v>9.566666666666666</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1214,10 +1274,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>147.0333333333333</v>
+        <v>38.93333333333333</v>
       </c>
       <c r="C21">
-        <v>147.6</v>
+        <v>11.83333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1225,10 +1285,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>1.5</v>
+        <v>241.5666666666667</v>
       </c>
       <c r="C22">
-        <v>1.2</v>
+        <v>149.3666666666667</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1236,10 +1296,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>244.6</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>149.2666666666667</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1247,10 +1307,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="1">
-        <v>1.25</v>
+        <v>26.96666666666667</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>16.83333333333333</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1258,10 +1318,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>1.375</v>
+        <v>1.444444444444444</v>
       </c>
       <c r="C25">
-        <v>1.25</v>
+        <v>1.285714285714286</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1272,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1280,10 +1340,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="1">
-        <v>13.9</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>13.33333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1291,10 +1351,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="1">
-        <v>9.266666666666667</v>
+        <v>1.25</v>
       </c>
       <c r="C28">
-        <v>5.066666666666666</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1302,10 +1362,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="1">
-        <v>2.12</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1313,10 +1373,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="1">
-        <v>10.36666666666667</v>
+        <v>31.7</v>
       </c>
       <c r="C30">
-        <v>9.4</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1324,10 +1384,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="1">
-        <v>1.333333333333333</v>
+        <v>6.068965517241379</v>
       </c>
       <c r="C31">
-        <v>1.333333333333333</v>
+        <v>4.166666666666667</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1335,10 +1395,10 @@
         <v>33</v>
       </c>
       <c r="B32" s="1">
-        <v>7</v>
+        <v>2.235294117647059</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1346,10 +1406,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="1">
-        <v>7.733333333333333</v>
+        <v>27.76666666666667</v>
       </c>
       <c r="C33">
-        <v>4.433333333333334</v>
+        <v>9.666666666666666</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1357,10 +1417,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="1">
-        <v>19.36666666666667</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>14.33333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1368,10 +1428,10 @@
         <v>36</v>
       </c>
       <c r="B35" s="1">
-        <v>2.105263157894737</v>
+        <v>1.125</v>
       </c>
       <c r="C35">
-        <v>1.428571428571429</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1379,10 +1439,10 @@
         <v>37</v>
       </c>
       <c r="B36" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1390,10 +1450,10 @@
         <v>38</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1401,10 +1461,10 @@
         <v>39</v>
       </c>
       <c r="B38" s="1">
-        <v>1</v>
+        <v>33.4</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1412,10 +1472,10 @@
         <v>40</v>
       </c>
       <c r="B39" s="1">
-        <v>4.966666666666667</v>
+        <v>1.846153846153846</v>
       </c>
       <c r="C39">
-        <v>4.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1423,10 +1483,10 @@
         <v>41</v>
       </c>
       <c r="B40" s="1">
-        <v>2.64</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C40">
-        <v>1.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1434,10 +1494,10 @@
         <v>42</v>
       </c>
       <c r="B41" s="1">
-        <v>2.44</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1445,10 +1505,10 @@
         <v>43</v>
       </c>
       <c r="B42" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1456,10 +1516,10 @@
         <v>44</v>
       </c>
       <c r="B43" s="1">
-        <v>2.32</v>
+        <v>19.46666666666667</v>
       </c>
       <c r="C43">
-        <v>1.75</v>
+        <v>4.233333333333333</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1467,10 +1527,10 @@
         <v>45</v>
       </c>
       <c r="B44" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>1.692307692307692</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1478,10 +1538,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="1">
-        <v>4.571428571428571</v>
+        <v>1.842105263157895</v>
       </c>
       <c r="C45">
-        <v>2.684210526315789</v>
+        <v>1.692307692307692</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1489,10 +1549,10 @@
         <v>47</v>
       </c>
       <c r="B46" s="1">
-        <v>10.5</v>
+        <v>1</v>
       </c>
       <c r="C46">
-        <v>10.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1500,10 +1560,10 @@
         <v>48</v>
       </c>
       <c r="B47" s="1">
-        <v>1.708333333333333</v>
+        <v>1.944444444444444</v>
       </c>
       <c r="C47">
-        <v>1.545454545454545</v>
+        <v>1.416666666666667</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1511,10 +1571,10 @@
         <v>49</v>
       </c>
       <c r="B48" s="1">
-        <v>3.689655172413793</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>4.466666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1522,10 +1582,10 @@
         <v>50</v>
       </c>
       <c r="B49" s="1">
-        <v>1.608695652173913</v>
+        <v>3.68</v>
       </c>
       <c r="C49">
-        <v>1.428571428571429</v>
+        <v>1.789473684210526</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1533,10 +1593,10 @@
         <v>51</v>
       </c>
       <c r="B50" s="1">
-        <v>1.25</v>
+        <v>23.7</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1547,7 +1607,7 @@
         <v>1.5</v>
       </c>
       <c r="C51">
-        <v>1.222222222222222</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1555,7 +1615,7 @@
         <v>53</v>
       </c>
       <c r="B52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1566,10 +1626,10 @@
         <v>54</v>
       </c>
       <c r="B53" s="1">
-        <v>2.269230769230769</v>
+        <v>15.26666666666667</v>
       </c>
       <c r="C53">
-        <v>1.5625</v>
+        <v>4.733333333333333</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1577,10 +1637,10 @@
         <v>55</v>
       </c>
       <c r="B54" s="1">
-        <v>1</v>
+        <v>1.1875</v>
       </c>
       <c r="C54">
-        <v>1.25</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1588,7 +1648,7 @@
         <v>56</v>
       </c>
       <c r="B55" s="1">
-        <v>1.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1599,10 +1659,10 @@
         <v>57</v>
       </c>
       <c r="B56" s="1">
-        <v>1.739130434782609</v>
+        <v>1.277777777777778</v>
       </c>
       <c r="C56">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1610,10 +1670,10 @@
         <v>58</v>
       </c>
       <c r="B57" s="1">
-        <v>1.583333333333333</v>
+        <v>1.25</v>
       </c>
       <c r="C57">
-        <v>1.545454545454545</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1621,10 +1681,10 @@
         <v>59</v>
       </c>
       <c r="B58" s="1">
-        <v>28.56666666666667</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>31.63333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1632,10 +1692,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="1">
-        <v>1.4</v>
+        <v>2.315789473684211</v>
       </c>
       <c r="C59">
-        <v>1.142857142857143</v>
+        <v>1.461538461538461</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1643,10 +1703,10 @@
         <v>61</v>
       </c>
       <c r="B60" s="1">
-        <v>2.076923076923077</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="C60">
-        <v>1.470588235294118</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1654,10 +1714,10 @@
         <v>62</v>
       </c>
       <c r="B61" s="1">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1665,10 +1725,10 @@
         <v>63</v>
       </c>
       <c r="B62" s="1">
-        <v>1</v>
+        <v>1.611111111111111</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1676,7 +1736,7 @@
         <v>64</v>
       </c>
       <c r="B63" s="1">
-        <v>1</v>
+        <v>1.5625</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -1687,10 +1747,10 @@
         <v>65</v>
       </c>
       <c r="B64" s="1">
-        <v>4.620689655172414</v>
+        <v>49.26666666666667</v>
       </c>
       <c r="C64">
-        <v>2.103448275862069</v>
+        <v>32.06666666666667</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1698,10 +1758,10 @@
         <v>66</v>
       </c>
       <c r="B65" s="1">
-        <v>6.2</v>
+        <v>1.444444444444444</v>
       </c>
       <c r="C65">
-        <v>6.433333333333334</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1709,10 +1769,10 @@
         <v>67</v>
       </c>
       <c r="B66" s="1">
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="C66">
-        <v>1.222222222222222</v>
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1720,10 +1780,10 @@
         <v>68</v>
       </c>
       <c r="B67" s="1">
-        <v>8.033333333333333</v>
+        <v>1</v>
       </c>
       <c r="C67">
-        <v>9.233333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1731,10 +1791,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="1">
-        <v>2.538461538461538</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>1.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1742,10 +1802,10 @@
         <v>70</v>
       </c>
       <c r="B69" s="1">
-        <v>1.739130434782609</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>1.454545454545455</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1753,10 +1813,10 @@
         <v>71</v>
       </c>
       <c r="B70" s="1">
-        <v>3.2</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="C70">
-        <v>2.25</v>
+        <v>1.956521739130435</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1764,10 +1824,10 @@
         <v>72</v>
       </c>
       <c r="B71" s="1">
-        <v>4.928571428571429</v>
+        <v>1</v>
       </c>
       <c r="C71">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1775,10 +1835,10 @@
         <v>73</v>
       </c>
       <c r="B72" s="1">
-        <v>3.714285714285714</v>
+        <v>1.277777777777778</v>
       </c>
       <c r="C72">
-        <v>1.863636363636364</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1786,10 +1846,10 @@
         <v>74</v>
       </c>
       <c r="B73" s="1">
-        <v>1.2</v>
+        <v>23.66666666666667</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>10.13333333333333</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1797,10 +1857,10 @@
         <v>75</v>
       </c>
       <c r="B74" s="1">
-        <v>50</v>
+        <v>2.72</v>
       </c>
       <c r="C74">
-        <v>48.96666666666667</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1808,10 +1868,10 @@
         <v>76</v>
       </c>
       <c r="B75" s="1">
-        <v>1.25</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1819,10 +1879,10 @@
         <v>77</v>
       </c>
       <c r="B76" s="1">
-        <v>1.708333333333333</v>
+        <v>2.722222222222222</v>
       </c>
       <c r="C76">
-        <v>1.375</v>
+        <v>1.583333333333333</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1830,10 +1890,10 @@
         <v>78</v>
       </c>
       <c r="B77" s="1">
-        <v>1</v>
+        <v>4.32</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>2.105263157894737</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1841,10 +1901,10 @@
         <v>79</v>
       </c>
       <c r="B78" s="1">
-        <v>3.24</v>
+        <v>2.5</v>
       </c>
       <c r="C78">
-        <v>2.230769230769231</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1852,10 +1912,10 @@
         <v>80</v>
       </c>
       <c r="B79" s="1">
-        <v>1.904761904761905</v>
+        <v>1</v>
       </c>
       <c r="C79">
-        <v>1.375</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1874,10 +1934,10 @@
         <v>82</v>
       </c>
       <c r="B81" s="1">
-        <v>15.9</v>
+        <v>71.3</v>
       </c>
       <c r="C81">
-        <v>7.733333333333333</v>
+        <v>48.93333333333333</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1885,7 +1945,7 @@
         <v>83</v>
       </c>
       <c r="B82" s="1">
-        <v>1.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -1896,10 +1956,10 @@
         <v>84</v>
       </c>
       <c r="B83" s="1">
-        <v>1</v>
+        <v>1.882352941176471</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>1.142857142857143</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1907,10 +1967,10 @@
         <v>85</v>
       </c>
       <c r="B84" s="1">
-        <v>1.142857142857143</v>
+        <v>1</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1918,10 +1978,10 @@
         <v>86</v>
       </c>
       <c r="B85" s="1">
-        <v>1.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1929,10 +1989,10 @@
         <v>87</v>
       </c>
       <c r="B86" s="1">
-        <v>2.423076923076923</v>
+        <v>2.777777777777778</v>
       </c>
       <c r="C86">
-        <v>1.833333333333333</v>
+        <v>1.583333333333333</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1940,10 +2000,10 @@
         <v>88</v>
       </c>
       <c r="B87" s="1">
-        <v>1.2</v>
+        <v>1.444444444444444</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1951,10 +2011,10 @@
         <v>89</v>
       </c>
       <c r="B88" s="1">
-        <v>4.633333333333334</v>
+        <v>1</v>
       </c>
       <c r="C88">
-        <v>4.066666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1962,10 +2022,10 @@
         <v>90</v>
       </c>
       <c r="B89" s="1">
-        <v>2.592592592592593</v>
+        <v>11.3</v>
       </c>
       <c r="C89">
-        <v>1.611111111111111</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1973,10 +2033,10 @@
         <v>91</v>
       </c>
       <c r="B90" s="1">
-        <v>18.36666666666667</v>
+        <v>1</v>
       </c>
       <c r="C90">
-        <v>8.966666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1984,7 +2044,7 @@
         <v>92</v>
       </c>
       <c r="B91" s="1">
-        <v>1.333333333333333</v>
+        <v>2.259259259259259</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -1995,10 +2055,10 @@
         <v>93</v>
       </c>
       <c r="B92" s="1">
-        <v>1.818181818181818</v>
+        <v>1</v>
       </c>
       <c r="C92">
-        <v>1.636363636363636</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2006,10 +2066,10 @@
         <v>94</v>
       </c>
       <c r="B93" s="1">
-        <v>26.83333333333333</v>
+        <v>0</v>
       </c>
       <c r="C93">
-        <v>23.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2017,10 +2077,10 @@
         <v>95</v>
       </c>
       <c r="B94" s="1">
-        <v>13.43333333333333</v>
+        <v>2.625</v>
       </c>
       <c r="C94">
-        <v>9.633333333333333</v>
+        <v>1.444444444444444</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2028,10 +2088,10 @@
         <v>96</v>
       </c>
       <c r="B95" s="1">
-        <v>6.133333333333334</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="C95">
-        <v>2.931034482758621</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2039,10 +2099,10 @@
         <v>97</v>
       </c>
       <c r="B96" s="1">
-        <v>1.4</v>
+        <v>16.43333333333333</v>
       </c>
       <c r="C96">
-        <v>1.142857142857143</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2050,10 +2110,10 @@
         <v>98</v>
       </c>
       <c r="B97" s="1">
-        <v>1.470588235294118</v>
+        <v>2.375</v>
       </c>
       <c r="C97">
-        <v>1.142857142857143</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2061,10 +2121,10 @@
         <v>99</v>
       </c>
       <c r="B98" s="1">
-        <v>3.310344827586207</v>
+        <v>34</v>
       </c>
       <c r="C98">
-        <v>2.866666666666667</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2072,7 +2132,7 @@
         <v>100</v>
       </c>
       <c r="B99" s="1">
-        <v>1</v>
+        <v>1.272727272727273</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -2083,10 +2143,10 @@
         <v>101</v>
       </c>
       <c r="B100" s="1">
-        <v>1.2</v>
+        <v>2.117647058823529</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>1.222222222222222</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2094,10 +2154,10 @@
         <v>102</v>
       </c>
       <c r="B101" s="1">
-        <v>31.66666666666667</v>
+        <v>40</v>
       </c>
       <c r="C101">
-        <v>34.76666666666667</v>
+        <v>22.93333333333333</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2105,10 +2165,10 @@
         <v>103</v>
       </c>
       <c r="B102" s="1">
-        <v>1.153846153846154</v>
+        <v>21.36666666666667</v>
       </c>
       <c r="C102">
-        <v>1.142857142857143</v>
+        <v>9.466666666666667</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2116,10 +2176,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="1">
-        <v>12.58620689655172</v>
+        <v>6.433333333333334</v>
       </c>
       <c r="C103">
-        <v>6.4</v>
+        <v>2.827586206896552</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2127,10 +2187,10 @@
         <v>105</v>
       </c>
       <c r="B104" s="1">
-        <v>6.2</v>
+        <v>1.444444444444444</v>
       </c>
       <c r="C104">
-        <v>5.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2138,10 +2198,10 @@
         <v>106</v>
       </c>
       <c r="B105" s="1">
-        <v>1.91304347826087</v>
+        <v>1.791666666666667</v>
       </c>
       <c r="C105">
-        <v>1.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2149,10 +2209,10 @@
         <v>107</v>
       </c>
       <c r="B106" s="1">
-        <v>5.607142857142857</v>
+        <v>1</v>
       </c>
       <c r="C106">
-        <v>3.227272727272727</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2160,10 +2220,10 @@
         <v>108</v>
       </c>
       <c r="B107" s="1">
-        <v>1.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2171,10 +2231,10 @@
         <v>109</v>
       </c>
       <c r="B108" s="1">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>36.26666666666667</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2182,10 +2242,10 @@
         <v>110</v>
       </c>
       <c r="B109" s="1">
-        <v>1.608695652173913</v>
+        <v>1.388888888888889</v>
       </c>
       <c r="C109">
-        <v>1.545454545454545</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2193,10 +2253,10 @@
         <v>111</v>
       </c>
       <c r="B110" s="1">
-        <v>1</v>
+        <v>8.758620689655173</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>4.923076923076923</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2204,10 +2264,10 @@
         <v>112</v>
       </c>
       <c r="B111" s="1">
-        <v>4.607142857142857</v>
+        <v>1</v>
       </c>
       <c r="C111">
-        <v>2.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2215,10 +2275,10 @@
         <v>113</v>
       </c>
       <c r="B112" s="1">
-        <v>10.93333333333333</v>
+        <v>19.23333333333333</v>
       </c>
       <c r="C112">
-        <v>8.066666666666666</v>
+        <v>5.466666666666667</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2226,10 +2286,10 @@
         <v>114</v>
       </c>
       <c r="B113" s="1">
-        <v>1.117647058823529</v>
+        <v>2.25</v>
       </c>
       <c r="C113">
-        <v>1.4</v>
+        <v>1.166666666666667</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2237,10 +2297,10 @@
         <v>115</v>
       </c>
       <c r="B114" s="1">
-        <v>1</v>
+        <v>5.583333333333333</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2248,10 +2308,10 @@
         <v>116</v>
       </c>
       <c r="B115" s="1">
-        <v>2.56</v>
+        <v>1</v>
       </c>
       <c r="C115">
-        <v>1.8125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2259,10 +2319,10 @@
         <v>117</v>
       </c>
       <c r="B116" s="1">
-        <v>1.111111111111111</v>
+        <v>1</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2270,7 +2330,7 @@
         <v>118</v>
       </c>
       <c r="B117" s="1">
-        <v>1.2</v>
+        <v>1.4375</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -2281,7 +2341,7 @@
         <v>119</v>
       </c>
       <c r="B118" s="1">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -2292,10 +2352,10 @@
         <v>120</v>
       </c>
       <c r="B119" s="1">
-        <v>1.782608695652174</v>
+        <v>4</v>
       </c>
       <c r="C119">
-        <v>1.454545454545455</v>
+        <v>1.888888888888889</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2303,10 +2363,10 @@
         <v>121</v>
       </c>
       <c r="B120" s="1">
-        <v>1</v>
+        <v>24.76666666666667</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>8.233333333333333</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2314,10 +2374,10 @@
         <v>122</v>
       </c>
       <c r="B121" s="1">
-        <v>1.625</v>
+        <v>1.357142857142857</v>
       </c>
       <c r="C121">
-        <v>1.176470588235294</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2328,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2336,10 +2396,10 @@
         <v>124</v>
       </c>
       <c r="B123" s="1">
-        <v>1.4</v>
+        <v>1.947368421052632</v>
       </c>
       <c r="C123">
-        <v>1.142857142857143</v>
+        <v>1.692307692307692</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2347,10 +2407,10 @@
         <v>125</v>
       </c>
       <c r="B124" s="1">
-        <v>7.866666666666666</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="C124">
-        <v>4.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2358,10 +2418,10 @@
         <v>126</v>
       </c>
       <c r="B125" s="1">
-        <v>14.2</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="C125">
-        <v>8.566666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2369,7 +2429,7 @@
         <v>127</v>
       </c>
       <c r="B126" s="1">
-        <v>1.2</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -2380,10 +2440,10 @@
         <v>128</v>
       </c>
       <c r="B127" s="1">
-        <v>1.739130434782609</v>
+        <v>1.2</v>
       </c>
       <c r="C127">
-        <v>1.454545454545455</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2394,7 +2454,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="C128">
-        <v>1.833333333333333</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2402,10 +2462,10 @@
         <v>130</v>
       </c>
       <c r="B129" s="1">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="C129">
-        <v>1.166666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2413,10 +2473,10 @@
         <v>131</v>
       </c>
       <c r="B130" s="1">
-        <v>4.428571428571429</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="C130">
-        <v>2.363636363636364</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2427,7 +2487,7 @@
         <v>1</v>
       </c>
       <c r="C131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2435,10 +2495,10 @@
         <v>133</v>
       </c>
       <c r="B132" s="1">
-        <v>1.230769230769231</v>
+        <v>1</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2446,10 +2506,10 @@
         <v>134</v>
       </c>
       <c r="B133" s="1">
-        <v>9.333333333333334</v>
+        <v>1.444444444444444</v>
       </c>
       <c r="C133">
-        <v>8.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2457,10 +2517,10 @@
         <v>135</v>
       </c>
       <c r="B134" s="1">
-        <v>2.153846153846154</v>
+        <v>6.4</v>
       </c>
       <c r="C134">
-        <v>1.5</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2468,10 +2528,10 @@
         <v>136</v>
       </c>
       <c r="B135" s="1">
-        <v>1</v>
+        <v>12.36666666666667</v>
       </c>
       <c r="C135">
-        <v>1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2479,10 +2539,10 @@
         <v>137</v>
       </c>
       <c r="B136" s="1">
-        <v>5.666666666666667</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="C136">
-        <v>5.633333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2490,10 +2550,10 @@
         <v>138</v>
       </c>
       <c r="B137" s="1">
-        <v>2.384615384615385</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C137">
-        <v>1.588235294117647</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2501,10 +2561,10 @@
         <v>139</v>
       </c>
       <c r="B138" s="1">
-        <v>1.652173913043478</v>
+        <v>1.25</v>
       </c>
       <c r="C138">
-        <v>1.545454545454545</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2512,10 +2572,10 @@
         <v>140</v>
       </c>
       <c r="B139" s="1">
-        <v>5.033333333333333</v>
+        <v>1.2</v>
       </c>
       <c r="C139">
-        <v>2.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2523,10 +2583,10 @@
         <v>141</v>
       </c>
       <c r="B140" s="1">
-        <v>1.545454545454545</v>
+        <v>4.133333333333334</v>
       </c>
       <c r="C140">
-        <v>1.222222222222222</v>
+        <v>1.421052631578947</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2534,10 +2594,10 @@
         <v>142</v>
       </c>
       <c r="B141" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C141">
-        <v>3.448275862068965</v>
+        <v>1.842105263157895</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2545,10 +2605,10 @@
         <v>143</v>
       </c>
       <c r="B142" s="1">
-        <v>16.26666666666667</v>
+        <v>4.2</v>
       </c>
       <c r="C142">
-        <v>11.3</v>
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2556,7 +2616,7 @@
         <v>144</v>
       </c>
       <c r="B143" s="1">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -2567,10 +2627,10 @@
         <v>145</v>
       </c>
       <c r="B144" s="1">
-        <v>12.83333333333333</v>
+        <v>25.16666666666667</v>
       </c>
       <c r="C144">
-        <v>7.2</v>
+        <v>8.566666666666666</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2578,10 +2638,10 @@
         <v>146</v>
       </c>
       <c r="B145" s="1">
-        <v>1</v>
+        <v>2.166666666666667</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2600,10 +2660,10 @@
         <v>148</v>
       </c>
       <c r="B147" s="1">
-        <v>3.689655172413793</v>
+        <v>19.46666666666667</v>
       </c>
       <c r="C147">
-        <v>4.333333333333333</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2611,10 +2671,10 @@
         <v>149</v>
       </c>
       <c r="B148" s="1">
-        <v>1</v>
+        <v>2.190476190476191</v>
       </c>
       <c r="C148">
-        <v>1</v>
+        <v>1.466666666666667</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2622,10 +2682,10 @@
         <v>150</v>
       </c>
       <c r="B149" s="1">
-        <v>3.2</v>
+        <v>1.4375</v>
       </c>
       <c r="C149">
-        <v>2.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2633,10 +2693,10 @@
         <v>151</v>
       </c>
       <c r="B150" s="1">
-        <v>37.1</v>
+        <v>9.5</v>
       </c>
       <c r="C150">
-        <v>35.6</v>
+        <v>2.148148148148148</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2644,10 +2704,10 @@
         <v>152</v>
       </c>
       <c r="B151" s="1">
-        <v>26.16666666666667</v>
+        <v>1.277777777777778</v>
       </c>
       <c r="C151">
-        <v>17.4</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2655,10 +2715,10 @@
         <v>153</v>
       </c>
       <c r="B152" s="1">
-        <v>1</v>
+        <v>13.8</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>3.642857142857143</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2666,10 +2726,10 @@
         <v>154</v>
       </c>
       <c r="B153" s="1">
-        <v>39.8</v>
+        <v>29.96666666666667</v>
       </c>
       <c r="C153">
-        <v>40</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2677,10 +2737,10 @@
         <v>155</v>
       </c>
       <c r="B154" s="1">
-        <v>37.03333333333333</v>
+        <v>1</v>
       </c>
       <c r="C154">
-        <v>36.63333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2688,10 +2748,10 @@
         <v>156</v>
       </c>
       <c r="B155" s="1">
-        <v>1</v>
+        <v>16.93333333333333</v>
       </c>
       <c r="C155">
-        <v>1</v>
+        <v>6.433333333333334</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2699,10 +2759,10 @@
         <v>157</v>
       </c>
       <c r="B156" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C156">
-        <v>1.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2710,10 +2770,10 @@
         <v>158</v>
       </c>
       <c r="B157" s="1">
-        <v>2.12</v>
+        <v>1</v>
       </c>
       <c r="C157">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2721,10 +2781,10 @@
         <v>159</v>
       </c>
       <c r="B158" s="1">
-        <v>1</v>
+        <v>12.26666666666667</v>
       </c>
       <c r="C158">
-        <v>1</v>
+        <v>4.633333333333334</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2732,10 +2792,10 @@
         <v>160</v>
       </c>
       <c r="B159" s="1">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2743,10 +2803,10 @@
         <v>161</v>
       </c>
       <c r="B160" s="1">
-        <v>2.12</v>
+        <v>1</v>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2754,10 +2814,10 @@
         <v>162</v>
       </c>
       <c r="B161" s="1">
-        <v>2.56</v>
+        <v>2.722222222222222</v>
       </c>
       <c r="C161">
-        <v>2</v>
+        <v>1.583333333333333</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2765,10 +2825,10 @@
         <v>163</v>
       </c>
       <c r="B162" s="1">
-        <v>3.875</v>
+        <v>1</v>
       </c>
       <c r="C162">
-        <v>3.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2776,10 +2836,10 @@
         <v>164</v>
       </c>
       <c r="B163" s="1">
-        <v>1.333333333333333</v>
+        <v>56.56666666666667</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>35.23333333333333</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2787,10 +2847,10 @@
         <v>165</v>
       </c>
       <c r="B164" s="1">
-        <v>5.620689655172414</v>
+        <v>1</v>
       </c>
       <c r="C164">
-        <v>3.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2798,10 +2858,10 @@
         <v>166</v>
       </c>
       <c r="B165" s="1">
-        <v>1.333333333333333</v>
+        <v>63.4</v>
       </c>
       <c r="C165">
-        <v>1</v>
+        <v>40.96666666666667</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2809,10 +2869,10 @@
         <v>167</v>
       </c>
       <c r="B166" s="1">
-        <v>3.571428571428572</v>
+        <v>58.53333333333333</v>
       </c>
       <c r="C166">
-        <v>1.863636363636364</v>
+        <v>37.3</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2820,10 +2880,10 @@
         <v>168</v>
       </c>
       <c r="B167" s="1">
-        <v>3.266666666666667</v>
+        <v>1</v>
       </c>
       <c r="C167">
-        <v>1.958333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2831,10 +2891,10 @@
         <v>169</v>
       </c>
       <c r="B168" s="1">
-        <v>3.04</v>
+        <v>1.357142857142857</v>
       </c>
       <c r="C168">
-        <v>2.083333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2842,10 +2902,10 @@
         <v>170</v>
       </c>
       <c r="B169" s="1">
-        <v>1.25</v>
+        <v>2.214285714285714</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2853,10 +2913,10 @@
         <v>171</v>
       </c>
       <c r="B170" s="1">
-        <v>2.04</v>
+        <v>1</v>
       </c>
       <c r="C170">
-        <v>1.818181818181818</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2864,10 +2924,10 @@
         <v>172</v>
       </c>
       <c r="B171" s="1">
-        <v>3.111111111111111</v>
+        <v>1</v>
       </c>
       <c r="C171">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2875,10 +2935,10 @@
         <v>173</v>
       </c>
       <c r="B172" s="1">
-        <v>1.636363636363636</v>
+        <v>2.294117647058823</v>
       </c>
       <c r="C172">
-        <v>1.222222222222222</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2886,10 +2946,10 @@
         <v>174</v>
       </c>
       <c r="B173" s="1">
-        <v>1.666666666666667</v>
+        <v>2.777777777777778</v>
       </c>
       <c r="C173">
-        <v>1</v>
+        <v>1.363636363636364</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2897,10 +2957,10 @@
         <v>175</v>
       </c>
       <c r="B174" s="1">
-        <v>1.375</v>
+        <v>1</v>
       </c>
       <c r="C174">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2908,10 +2968,10 @@
         <v>176</v>
       </c>
       <c r="B175" s="1">
-        <v>2.52</v>
+        <v>2.266666666666667</v>
       </c>
       <c r="C175">
-        <v>1.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2919,10 +2979,10 @@
         <v>177</v>
       </c>
       <c r="B176" s="1">
-        <v>55.53333333333333</v>
+        <v>1</v>
       </c>
       <c r="C176">
-        <v>55.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2930,10 +2990,10 @@
         <v>178</v>
       </c>
       <c r="B177" s="1">
-        <v>1.0625</v>
+        <v>1</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2941,10 +3001,10 @@
         <v>179</v>
       </c>
       <c r="B178" s="1">
-        <v>1</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="C178">
-        <v>0</v>
+        <v>2.434782608695652</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2952,10 +3012,10 @@
         <v>180</v>
       </c>
       <c r="B179" s="1">
-        <v>2.392857142857143</v>
+        <v>1</v>
       </c>
       <c r="C179">
-        <v>1.368421052631579</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2963,10 +3023,10 @@
         <v>181</v>
       </c>
       <c r="B180" s="1">
-        <v>1</v>
+        <v>2.692307692307693</v>
       </c>
       <c r="C180">
-        <v>1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2974,10 +3034,10 @@
         <v>182</v>
       </c>
       <c r="B181" s="1">
-        <v>8.633333333333333</v>
+        <v>10.1</v>
       </c>
       <c r="C181">
-        <v>4.733333333333333</v>
+        <v>2.409090909090909</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2985,10 +3045,10 @@
         <v>183</v>
       </c>
       <c r="B182" s="1">
-        <v>2.043478260869565</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="C182">
-        <v>1.875</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2996,7 +3056,7 @@
         <v>184</v>
       </c>
       <c r="B183" s="1">
-        <v>1.473684210526316</v>
+        <v>1</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -3007,10 +3067,10 @@
         <v>185</v>
       </c>
       <c r="B184" s="1">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="C184">
-        <v>1.769230769230769</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3018,10 +3078,10 @@
         <v>186</v>
       </c>
       <c r="B185" s="1">
-        <v>1.083333333333333</v>
+        <v>2.117647058823529</v>
       </c>
       <c r="C185">
-        <v>1.333333333333333</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3029,10 +3089,10 @@
         <v>187</v>
       </c>
       <c r="B186" s="1">
-        <v>1.931034482758621</v>
+        <v>2.761904761904762</v>
       </c>
       <c r="C186">
-        <v>1.708333333333333</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3040,10 +3100,10 @@
         <v>188</v>
       </c>
       <c r="B187" s="1">
-        <v>1.545454545454545</v>
+        <v>1.125</v>
       </c>
       <c r="C187">
-        <v>1.222222222222222</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3051,10 +3111,10 @@
         <v>189</v>
       </c>
       <c r="B188" s="1">
-        <v>1.458333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C188">
-        <v>1.625</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3062,10 +3122,10 @@
         <v>190</v>
       </c>
       <c r="B189" s="1">
-        <v>1.368421052631579</v>
+        <v>1.5</v>
       </c>
       <c r="C189">
-        <v>1.285714285714286</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3073,10 +3133,10 @@
         <v>191</v>
       </c>
       <c r="B190" s="1">
-        <v>2.12</v>
+        <v>1.214285714285714</v>
       </c>
       <c r="C190">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3084,10 +3144,10 @@
         <v>192</v>
       </c>
       <c r="B191" s="1">
-        <v>1.782608695652174</v>
+        <v>1</v>
       </c>
       <c r="C191">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3095,10 +3155,10 @@
         <v>193</v>
       </c>
       <c r="B192" s="1">
-        <v>1.090909090909091</v>
+        <v>1.894736842105263</v>
       </c>
       <c r="C192">
-        <v>1</v>
+        <v>1.692307692307692</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3106,10 +3166,10 @@
         <v>194</v>
       </c>
       <c r="B193" s="1">
-        <v>1.782608695652174</v>
+        <v>78.96666666666667</v>
       </c>
       <c r="C193">
-        <v>1.454545454545455</v>
+        <v>54.7</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3117,10 +3177,10 @@
         <v>195</v>
       </c>
       <c r="B194" s="1">
-        <v>1.565217391304348</v>
+        <v>1.3</v>
       </c>
       <c r="C194">
-        <v>1.545454545454545</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3128,10 +3188,10 @@
         <v>196</v>
       </c>
       <c r="B195" s="1">
-        <v>1.307692307692308</v>
+        <v>1</v>
       </c>
       <c r="C195">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3139,10 +3199,10 @@
         <v>197</v>
       </c>
       <c r="B196" s="1">
-        <v>23.1</v>
+        <v>1</v>
       </c>
       <c r="C196">
-        <v>22.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3150,10 +3210,10 @@
         <v>198</v>
       </c>
       <c r="B197" s="1">
-        <v>1.333333333333333</v>
+        <v>9.766666666666667</v>
       </c>
       <c r="C197">
-        <v>1</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3161,10 +3221,230 @@
         <v>199</v>
       </c>
       <c r="B198" s="1">
-        <v>1.739130434782609</v>
+        <v>3.379310344827586</v>
       </c>
       <c r="C198">
-        <v>1.5</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B199" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="C199">
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B200" s="1">
+        <v>2.615384615384615</v>
+      </c>
+      <c r="C200">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B201" s="1">
+        <v>1.277777777777778</v>
+      </c>
+      <c r="C201">
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B202" s="1">
+        <v>1</v>
+      </c>
+      <c r="C202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B203" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C203">
+        <v>1.333333333333333</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B204" s="1">
+        <v>1.125</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B205" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="C205">
+        <v>2.115384615384615</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B206" s="1">
+        <v>1.277777777777778</v>
+      </c>
+      <c r="C206">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B207" s="1">
+        <v>1.625</v>
+      </c>
+      <c r="C207">
+        <v>1.444444444444444</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B208" s="1">
+        <v>1</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B209" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C209">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B210" s="1">
+        <v>2.235294117647059</v>
+      </c>
+      <c r="C210">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B211" s="1">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="C211">
+        <v>1.416666666666667</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B212" s="1">
+        <v>1.571428571428571</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B213" s="1">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="C213">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B214" s="1">
+        <v>1.461538461538461</v>
+      </c>
+      <c r="C214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B215" s="1">
+        <v>7.033333333333333</v>
+      </c>
+      <c r="C215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B216" s="1">
+        <v>40.33333333333334</v>
+      </c>
+      <c r="C216">
+        <v>22.03333333333333</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B217" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B218" s="1">
+        <v>1.611111111111111</v>
+      </c>
+      <c r="C218">
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "correcting error in top20"
This reverts commit 218c23ab125ffb198ae656c8644173250a696c48.
</commit_message>
<xml_diff>
--- a/results/example/rate.xlsx
+++ b/results/example/rate.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
-  <si>
-    <t>P9_ultra</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
+  <si>
+    <t>P9</t>
   </si>
   <si>
     <t>P9+BB_slnc</t>
@@ -31,12 +31,6 @@
     <t>BB_r</t>
   </si>
   <si>
-    <t>CIN-P9-1_l</t>
-  </si>
-  <si>
-    <t>CIN-P9-1_r</t>
-  </si>
-  <si>
     <t>DNa01_l</t>
   </si>
   <si>
@@ -73,27 +67,24 @@
     <t>MooDNg_l</t>
   </si>
   <si>
+    <t>P9-0DN1_l</t>
+  </si>
+  <si>
+    <t>P9-0DN1_r</t>
+  </si>
+  <si>
     <t>P9-cDN1_l</t>
   </si>
   <si>
     <t>P9-cDN1_r</t>
   </si>
   <si>
-    <t>P9-oDN1_l</t>
-  </si>
-  <si>
-    <t>P9-oDN1_r</t>
-  </si>
-  <si>
     <t>P9_l</t>
   </si>
   <si>
     <t>P9_r</t>
   </si>
   <si>
-    <t>neck motor neuron_r</t>
-  </si>
-  <si>
     <t>720575940604735660</t>
   </si>
   <si>
@@ -124,9 +115,6 @@
     <t>720575940606667868</t>
   </si>
   <si>
-    <t>720575940606852018</t>
-  </si>
-  <si>
     <t>720575940607641010</t>
   </si>
   <si>
@@ -157,7 +145,7 @@
     <t>720575940611206514</t>
   </si>
   <si>
-    <t>720575940611772514</t>
+    <t>720575940612629210</t>
   </si>
   <si>
     <t>720575940612766515</t>
@@ -175,9 +163,6 @@
     <t>720575940614963359</t>
   </si>
   <si>
-    <t>720575940615484063</t>
-  </si>
-  <si>
     <t>720575940615626562</t>
   </si>
   <si>
@@ -190,9 +175,6 @@
     <t>720575940615997919</t>
   </si>
   <si>
-    <t>720575940616018956</t>
-  </si>
-  <si>
     <t>720575940616566203</t>
   </si>
   <si>
@@ -232,7 +214,7 @@
     <t>720575940618156829</t>
   </si>
   <si>
-    <t>720575940618167579</t>
+    <t>720575940618165393</t>
   </si>
   <si>
     <t>720575940618177977</t>
@@ -259,9 +241,6 @@
     <t>720575940619681006</t>
   </si>
   <si>
-    <t>720575940619866027</t>
-  </si>
-  <si>
     <t>720575940619876884</t>
   </si>
   <si>
@@ -274,9 +253,6 @@
     <t>720575940620231590</t>
   </si>
   <si>
-    <t>720575940620250328</t>
-  </si>
-  <si>
     <t>720575940620282900</t>
   </si>
   <si>
@@ -337,6 +313,9 @@
     <t>720575940622933130</t>
   </si>
   <si>
+    <t>720575940622998627</t>
+  </si>
+  <si>
     <t>720575940623164515</t>
   </si>
   <si>
@@ -352,9 +331,6 @@
     <t>720575940624163303</t>
   </si>
   <si>
-    <t>720575940624231143</t>
-  </si>
-  <si>
     <t>720575940624336115</t>
   </si>
   <si>
@@ -394,9 +370,6 @@
     <t>720575940626210536</t>
   </si>
   <si>
-    <t>720575940626279486</t>
-  </si>
-  <si>
     <t>720575940626310960</t>
   </si>
   <si>
@@ -415,9 +388,6 @@
     <t>720575940626773523</t>
   </si>
   <si>
-    <t>720575940626812218</t>
-  </si>
-  <si>
     <t>720575940626829852</t>
   </si>
   <si>
@@ -433,9 +403,6 @@
     <t>720575940627348057</t>
   </si>
   <si>
-    <t>720575940627358853</t>
-  </si>
-  <si>
     <t>720575940627361157</t>
   </si>
   <si>
@@ -499,18 +466,15 @@
     <t>720575940630291767</t>
   </si>
   <si>
-    <t>720575940630808591</t>
-  </si>
-  <si>
     <t>720575940630931999</t>
   </si>
   <si>
-    <t>720575940631283267</t>
-  </si>
-  <si>
     <t>720575940631283512</t>
   </si>
   <si>
+    <t>720575940631715896</t>
+  </si>
+  <si>
     <t>720575940631721785</t>
   </si>
   <si>
@@ -541,18 +505,12 @@
     <t>720575940632943315</t>
   </si>
   <si>
-    <t>720575940632944339</t>
-  </si>
-  <si>
     <t>720575940632962786</t>
   </si>
   <si>
     <t>720575940633116256</t>
   </si>
   <si>
-    <t>720575940633270497</t>
-  </si>
-  <si>
     <t>720575940633308371</t>
   </si>
   <si>
@@ -571,18 +529,12 @@
     <t>720575940635170484</t>
   </si>
   <si>
-    <t>720575940635179359</t>
-  </si>
-  <si>
     <t>720575940635771316</t>
   </si>
   <si>
     <t>720575940635776760</t>
   </si>
   <si>
-    <t>720575940635937678</t>
-  </si>
-  <si>
     <t>720575940635942507</t>
   </si>
   <si>
@@ -592,9 +544,6 @@
     <t>720575940636879534</t>
   </si>
   <si>
-    <t>720575940636933751</t>
-  </si>
-  <si>
     <t>720575940637308605</t>
   </si>
   <si>
@@ -604,10 +553,7 @@
     <t>720575940638169917</t>
   </si>
   <si>
-    <t>720575940638196038</t>
-  </si>
-  <si>
-    <t>720575940638681917</t>
+    <t>720575940638664355</t>
   </si>
   <si>
     <t>720575940638989894</t>
@@ -625,9 +571,6 @@
     <t>720575940640696027</t>
   </si>
   <si>
-    <t>720575940641480949</t>
-  </si>
-  <si>
     <t>720575940641585627</t>
   </si>
   <si>
@@ -641,9 +584,6 @@
   </si>
   <si>
     <t>720575940644758308</t>
-  </si>
-  <si>
-    <t>720575940645047831</t>
   </si>
   <si>
     <t>720575940646126190</t>
@@ -1035,7 +975,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1068,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>109.5666666666667</v>
+        <v>109.7666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1079,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>113.6666666666667</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1087,10 +1027,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>13.9</v>
+        <v>28.16666666666667</v>
       </c>
       <c r="C4">
-        <v>3.714285714285714</v>
+        <v>16.33333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1098,10 +1038,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>21.66666666666667</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>6.3</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1109,10 +1049,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>42.63333333333333</v>
+        <v>27.43333333333333</v>
       </c>
       <c r="C6">
-        <v>15.86666666666667</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1120,10 +1060,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>34.13333333333333</v>
+        <v>10.53333333333333</v>
       </c>
       <c r="C7">
-        <v>11.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1131,10 +1071,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>37.76666666666667</v>
+        <v>29</v>
       </c>
       <c r="C8">
-        <v>14.8</v>
+        <v>18.6</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1142,10 +1082,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>16.3</v>
+        <v>22.83333333333333</v>
       </c>
       <c r="C9">
-        <v>5.366666666666666</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1153,10 +1093,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>29.53333333333333</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>17.76666666666667</v>
+        <v>6.133333333333334</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1164,10 +1104,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>26.66666666666667</v>
+        <v>8.233333333333333</v>
       </c>
       <c r="C11">
-        <v>10.7</v>
+        <v>4.466666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1175,10 +1115,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>17.16666666666667</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>6.166666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1186,10 +1126,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>16.8</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>1.421052631578947</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1197,10 +1137,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>2.931034482758621</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1208,10 +1148,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>13.8</v>
+        <v>5.6</v>
       </c>
       <c r="C15">
-        <v>1.578947368421053</v>
+        <v>2.133333333333333</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1219,10 +1159,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>1.333333333333333</v>
+        <v>20.73333333333333</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1230,10 +1170,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="1">
-        <v>10.53333333333333</v>
+        <v>25.9</v>
       </c>
       <c r="C17">
-        <v>2.5</v>
+        <v>12.36666666666667</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1241,10 +1181,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>27</v>
+        <v>22.4</v>
       </c>
       <c r="C18">
-        <v>10.36666666666667</v>
+        <v>10.66666666666667</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1252,10 +1192,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>13.16666666666667</v>
+        <v>13.8</v>
       </c>
       <c r="C19">
-        <v>5.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1263,10 +1203,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>35.26666666666667</v>
+        <v>151.9</v>
       </c>
       <c r="C20">
-        <v>9.566666666666666</v>
+        <v>149.2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1274,10 +1214,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>38.93333333333333</v>
+        <v>147.0333333333333</v>
       </c>
       <c r="C21">
-        <v>11.83333333333333</v>
+        <v>147.6</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1285,10 +1225,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>241.5666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="C22">
-        <v>149.3666666666667</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1296,10 +1236,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>244.6</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>149.2666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1307,10 +1247,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="1">
-        <v>26.96666666666667</v>
+        <v>1.25</v>
       </c>
       <c r="C24">
-        <v>16.83333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1318,10 +1258,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>1.444444444444444</v>
+        <v>1.375</v>
       </c>
       <c r="C25">
-        <v>1.285714285714286</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1332,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1340,10 +1280,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>13.9</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>13.33333333333333</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1351,10 +1291,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="1">
-        <v>1.25</v>
+        <v>9.266666666666667</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>5.066666666666666</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1362,10 +1302,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="1">
-        <v>1</v>
+        <v>2.12</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1373,10 +1313,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="1">
-        <v>31.7</v>
+        <v>10.36666666666667</v>
       </c>
       <c r="C30">
-        <v>13.8</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1384,10 +1324,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="1">
-        <v>6.068965517241379</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C31">
-        <v>4.166666666666667</v>
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1395,10 +1335,10 @@
         <v>33</v>
       </c>
       <c r="B32" s="1">
-        <v>2.235294117647059</v>
+        <v>7</v>
       </c>
       <c r="C32">
-        <v>1.3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1406,10 +1346,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="1">
-        <v>27.76666666666667</v>
+        <v>7.733333333333333</v>
       </c>
       <c r="C33">
-        <v>9.666666666666666</v>
+        <v>4.433333333333334</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1417,10 +1357,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="1">
-        <v>2</v>
+        <v>19.36666666666667</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>14.33333333333333</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1428,10 +1368,10 @@
         <v>36</v>
       </c>
       <c r="B35" s="1">
-        <v>1.125</v>
+        <v>2.105263157894737</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1.428571428571429</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1439,10 +1379,10 @@
         <v>37</v>
       </c>
       <c r="B36" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>3.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1450,10 +1390,10 @@
         <v>38</v>
       </c>
       <c r="B37" s="1">
-        <v>6.666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>4.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1461,10 +1401,10 @@
         <v>39</v>
       </c>
       <c r="B38" s="1">
-        <v>33.4</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>13.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1472,10 +1412,10 @@
         <v>40</v>
       </c>
       <c r="B39" s="1">
-        <v>1.846153846153846</v>
+        <v>4.966666666666667</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1483,10 +1423,10 @@
         <v>41</v>
       </c>
       <c r="B40" s="1">
-        <v>1.333333333333333</v>
+        <v>2.64</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1494,10 +1434,10 @@
         <v>42</v>
       </c>
       <c r="B41" s="1">
-        <v>1</v>
+        <v>2.44</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1505,10 +1445,10 @@
         <v>43</v>
       </c>
       <c r="B42" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1516,10 +1456,10 @@
         <v>44</v>
       </c>
       <c r="B43" s="1">
-        <v>19.46666666666667</v>
+        <v>2.32</v>
       </c>
       <c r="C43">
-        <v>4.233333333333333</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1527,10 +1467,10 @@
         <v>45</v>
       </c>
       <c r="B44" s="1">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>1.692307692307692</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1538,10 +1478,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="1">
-        <v>1.842105263157895</v>
+        <v>4.571428571428571</v>
       </c>
       <c r="C45">
-        <v>1.692307692307692</v>
+        <v>2.684210526315789</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1549,10 +1489,10 @@
         <v>47</v>
       </c>
       <c r="B46" s="1">
-        <v>1</v>
+        <v>10.5</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1560,10 +1500,10 @@
         <v>48</v>
       </c>
       <c r="B47" s="1">
-        <v>1.944444444444444</v>
+        <v>1.708333333333333</v>
       </c>
       <c r="C47">
-        <v>1.416666666666667</v>
+        <v>1.545454545454545</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1571,10 +1511,10 @@
         <v>49</v>
       </c>
       <c r="B48" s="1">
-        <v>1</v>
+        <v>3.689655172413793</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>4.466666666666667</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1582,10 +1522,10 @@
         <v>50</v>
       </c>
       <c r="B49" s="1">
-        <v>3.68</v>
+        <v>1.608695652173913</v>
       </c>
       <c r="C49">
-        <v>1.789473684210526</v>
+        <v>1.428571428571429</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1593,10 +1533,10 @@
         <v>51</v>
       </c>
       <c r="B50" s="1">
-        <v>23.7</v>
+        <v>1.25</v>
       </c>
       <c r="C50">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1607,7 +1547,7 @@
         <v>1.5</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>1.222222222222222</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1615,7 +1555,7 @@
         <v>53</v>
       </c>
       <c r="B52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1626,10 +1566,10 @@
         <v>54</v>
       </c>
       <c r="B53" s="1">
-        <v>15.26666666666667</v>
+        <v>2.269230769230769</v>
       </c>
       <c r="C53">
-        <v>4.733333333333333</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1637,10 +1577,10 @@
         <v>55</v>
       </c>
       <c r="B54" s="1">
-        <v>1.1875</v>
+        <v>1</v>
       </c>
       <c r="C54">
-        <v>1.4</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1648,7 +1588,7 @@
         <v>56</v>
       </c>
       <c r="B55" s="1">
-        <v>1</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1659,10 +1599,10 @@
         <v>57</v>
       </c>
       <c r="B56" s="1">
-        <v>1.277777777777778</v>
+        <v>1.739130434782609</v>
       </c>
       <c r="C56">
-        <v>1.1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1670,10 +1610,10 @@
         <v>58</v>
       </c>
       <c r="B57" s="1">
-        <v>1.25</v>
+        <v>1.583333333333333</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1.545454545454545</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1681,10 +1621,10 @@
         <v>59</v>
       </c>
       <c r="B58" s="1">
-        <v>1</v>
+        <v>28.56666666666667</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>31.63333333333333</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1692,10 +1632,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="1">
-        <v>2.315789473684211</v>
+        <v>1.4</v>
       </c>
       <c r="C59">
-        <v>1.461538461538461</v>
+        <v>1.142857142857143</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1703,10 +1643,10 @@
         <v>61</v>
       </c>
       <c r="B60" s="1">
-        <v>3.333333333333333</v>
+        <v>2.076923076923077</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>1.470588235294118</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1714,10 +1654,10 @@
         <v>62</v>
       </c>
       <c r="B61" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1725,10 +1665,10 @@
         <v>63</v>
       </c>
       <c r="B62" s="1">
-        <v>1.611111111111111</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1736,7 +1676,7 @@
         <v>64</v>
       </c>
       <c r="B63" s="1">
-        <v>1.5625</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -1747,10 +1687,10 @@
         <v>65</v>
       </c>
       <c r="B64" s="1">
-        <v>49.26666666666667</v>
+        <v>4.620689655172414</v>
       </c>
       <c r="C64">
-        <v>32.06666666666667</v>
+        <v>2.103448275862069</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1758,10 +1698,10 @@
         <v>66</v>
       </c>
       <c r="B65" s="1">
-        <v>1.444444444444444</v>
+        <v>6.2</v>
       </c>
       <c r="C65">
-        <v>1.2</v>
+        <v>6.433333333333334</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1769,10 +1709,10 @@
         <v>67</v>
       </c>
       <c r="B66" s="1">
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="C66">
-        <v>1.333333333333333</v>
+        <v>1.222222222222222</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1780,10 +1720,10 @@
         <v>68</v>
       </c>
       <c r="B67" s="1">
-        <v>1</v>
+        <v>8.033333333333333</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>9.233333333333333</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1791,10 +1731,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="1">
-        <v>1</v>
+        <v>2.538461538461538</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>1.666666666666667</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1802,10 +1742,10 @@
         <v>70</v>
       </c>
       <c r="B69" s="1">
-        <v>1</v>
+        <v>1.739130434782609</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>1.454545454545455</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1813,10 +1753,10 @@
         <v>71</v>
       </c>
       <c r="B70" s="1">
-        <v>8.300000000000001</v>
+        <v>3.2</v>
       </c>
       <c r="C70">
-        <v>1.956521739130435</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1824,10 +1764,10 @@
         <v>72</v>
       </c>
       <c r="B71" s="1">
-        <v>1</v>
+        <v>4.928571428571429</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1835,10 +1775,10 @@
         <v>73</v>
       </c>
       <c r="B72" s="1">
-        <v>1.277777777777778</v>
+        <v>3.714285714285714</v>
       </c>
       <c r="C72">
-        <v>1.1</v>
+        <v>1.863636363636364</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1846,10 +1786,10 @@
         <v>74</v>
       </c>
       <c r="B73" s="1">
-        <v>23.66666666666667</v>
+        <v>1.2</v>
       </c>
       <c r="C73">
-        <v>10.13333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1857,10 +1797,10 @@
         <v>75</v>
       </c>
       <c r="B74" s="1">
-        <v>2.72</v>
+        <v>50</v>
       </c>
       <c r="C74">
-        <v>1.625</v>
+        <v>48.96666666666667</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1868,10 +1808,10 @@
         <v>76</v>
       </c>
       <c r="B75" s="1">
-        <v>1.666666666666667</v>
+        <v>1.25</v>
       </c>
       <c r="C75">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1879,10 +1819,10 @@
         <v>77</v>
       </c>
       <c r="B76" s="1">
-        <v>2.722222222222222</v>
+        <v>1.708333333333333</v>
       </c>
       <c r="C76">
-        <v>1.583333333333333</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1890,10 +1830,10 @@
         <v>78</v>
       </c>
       <c r="B77" s="1">
-        <v>4.32</v>
+        <v>1</v>
       </c>
       <c r="C77">
-        <v>2.105263157894737</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1901,10 +1841,10 @@
         <v>79</v>
       </c>
       <c r="B78" s="1">
-        <v>2.5</v>
+        <v>3.24</v>
       </c>
       <c r="C78">
-        <v>1.75</v>
+        <v>2.230769230769231</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1912,10 +1852,10 @@
         <v>80</v>
       </c>
       <c r="B79" s="1">
-        <v>1</v>
+        <v>1.904761904761905</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1934,10 +1874,10 @@
         <v>82</v>
       </c>
       <c r="B81" s="1">
-        <v>71.3</v>
+        <v>15.9</v>
       </c>
       <c r="C81">
-        <v>48.93333333333333</v>
+        <v>7.733333333333333</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1945,7 +1885,7 @@
         <v>83</v>
       </c>
       <c r="B82" s="1">
-        <v>1</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -1956,10 +1896,10 @@
         <v>84</v>
       </c>
       <c r="B83" s="1">
-        <v>1.882352941176471</v>
+        <v>1</v>
       </c>
       <c r="C83">
-        <v>1.142857142857143</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1967,10 +1907,10 @@
         <v>85</v>
       </c>
       <c r="B84" s="1">
-        <v>1</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1978,10 +1918,10 @@
         <v>86</v>
       </c>
       <c r="B85" s="1">
-        <v>1</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1989,10 +1929,10 @@
         <v>87</v>
       </c>
       <c r="B86" s="1">
-        <v>2.777777777777778</v>
+        <v>2.423076923076923</v>
       </c>
       <c r="C86">
-        <v>1.583333333333333</v>
+        <v>1.833333333333333</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2000,10 +1940,10 @@
         <v>88</v>
       </c>
       <c r="B87" s="1">
-        <v>1.444444444444444</v>
+        <v>1.2</v>
       </c>
       <c r="C87">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2011,10 +1951,10 @@
         <v>89</v>
       </c>
       <c r="B88" s="1">
-        <v>1</v>
+        <v>4.633333333333334</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>4.066666666666666</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2022,10 +1962,10 @@
         <v>90</v>
       </c>
       <c r="B89" s="1">
-        <v>11.3</v>
+        <v>2.592592592592593</v>
       </c>
       <c r="C89">
-        <v>6.666666666666667</v>
+        <v>1.611111111111111</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2033,10 +1973,10 @@
         <v>91</v>
       </c>
       <c r="B90" s="1">
-        <v>1</v>
+        <v>18.36666666666667</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>8.966666666666667</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2044,7 +1984,7 @@
         <v>92</v>
       </c>
       <c r="B91" s="1">
-        <v>2.259259259259259</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -2055,10 +1995,10 @@
         <v>93</v>
       </c>
       <c r="B92" s="1">
-        <v>1</v>
+        <v>1.818181818181818</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>1.636363636363636</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2066,10 +2006,10 @@
         <v>94</v>
       </c>
       <c r="B93" s="1">
-        <v>0</v>
+        <v>26.83333333333333</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2077,10 +2017,10 @@
         <v>95</v>
       </c>
       <c r="B94" s="1">
-        <v>2.625</v>
+        <v>13.43333333333333</v>
       </c>
       <c r="C94">
-        <v>1.444444444444444</v>
+        <v>9.633333333333333</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2088,10 +2028,10 @@
         <v>96</v>
       </c>
       <c r="B95" s="1">
-        <v>1.166666666666667</v>
+        <v>6.133333333333334</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>2.931034482758621</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2099,10 +2039,10 @@
         <v>97</v>
       </c>
       <c r="B96" s="1">
-        <v>16.43333333333333</v>
+        <v>1.4</v>
       </c>
       <c r="C96">
-        <v>4.7</v>
+        <v>1.142857142857143</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2110,10 +2050,10 @@
         <v>98</v>
       </c>
       <c r="B97" s="1">
-        <v>2.375</v>
+        <v>1.470588235294118</v>
       </c>
       <c r="C97">
-        <v>1.5</v>
+        <v>1.142857142857143</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2121,10 +2061,10 @@
         <v>99</v>
       </c>
       <c r="B98" s="1">
-        <v>34</v>
+        <v>3.310344827586207</v>
       </c>
       <c r="C98">
-        <v>8.800000000000001</v>
+        <v>2.866666666666667</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2132,7 +2072,7 @@
         <v>100</v>
       </c>
       <c r="B99" s="1">
-        <v>1.272727272727273</v>
+        <v>1</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -2143,10 +2083,10 @@
         <v>101</v>
       </c>
       <c r="B100" s="1">
-        <v>2.117647058823529</v>
+        <v>1.2</v>
       </c>
       <c r="C100">
-        <v>1.222222222222222</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2154,10 +2094,10 @@
         <v>102</v>
       </c>
       <c r="B101" s="1">
-        <v>40</v>
+        <v>31.66666666666667</v>
       </c>
       <c r="C101">
-        <v>22.93333333333333</v>
+        <v>34.76666666666667</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2165,10 +2105,10 @@
         <v>103</v>
       </c>
       <c r="B102" s="1">
-        <v>21.36666666666667</v>
+        <v>1.153846153846154</v>
       </c>
       <c r="C102">
-        <v>9.466666666666667</v>
+        <v>1.142857142857143</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2176,10 +2116,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="1">
-        <v>6.433333333333334</v>
+        <v>12.58620689655172</v>
       </c>
       <c r="C103">
-        <v>2.827586206896552</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2187,10 +2127,10 @@
         <v>105</v>
       </c>
       <c r="B104" s="1">
-        <v>1.444444444444444</v>
+        <v>6.2</v>
       </c>
       <c r="C104">
-        <v>1.2</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2198,10 +2138,10 @@
         <v>106</v>
       </c>
       <c r="B105" s="1">
-        <v>1.791666666666667</v>
+        <v>1.91304347826087</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2209,10 +2149,10 @@
         <v>107</v>
       </c>
       <c r="B106" s="1">
-        <v>1</v>
+        <v>5.607142857142857</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>3.227272727272727</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2220,10 +2160,10 @@
         <v>108</v>
       </c>
       <c r="B107" s="1">
-        <v>1</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2231,10 +2171,10 @@
         <v>109</v>
       </c>
       <c r="B108" s="1">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C108">
-        <v>36.26666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2242,10 +2182,10 @@
         <v>110</v>
       </c>
       <c r="B109" s="1">
-        <v>1.388888888888889</v>
+        <v>1.608695652173913</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>1.545454545454545</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2253,10 +2193,10 @@
         <v>111</v>
       </c>
       <c r="B110" s="1">
-        <v>8.758620689655173</v>
+        <v>1</v>
       </c>
       <c r="C110">
-        <v>4.923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2264,10 +2204,10 @@
         <v>112</v>
       </c>
       <c r="B111" s="1">
-        <v>1</v>
+        <v>4.607142857142857</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2275,10 +2215,10 @@
         <v>113</v>
       </c>
       <c r="B112" s="1">
-        <v>19.23333333333333</v>
+        <v>10.93333333333333</v>
       </c>
       <c r="C112">
-        <v>5.466666666666667</v>
+        <v>8.066666666666666</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2286,10 +2226,10 @@
         <v>114</v>
       </c>
       <c r="B113" s="1">
-        <v>2.25</v>
+        <v>1.117647058823529</v>
       </c>
       <c r="C113">
-        <v>1.166666666666667</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2297,10 +2237,10 @@
         <v>115</v>
       </c>
       <c r="B114" s="1">
-        <v>5.583333333333333</v>
+        <v>1</v>
       </c>
       <c r="C114">
-        <v>2.35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2308,10 +2248,10 @@
         <v>116</v>
       </c>
       <c r="B115" s="1">
-        <v>1</v>
+        <v>2.56</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>1.8125</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2319,10 +2259,10 @@
         <v>117</v>
       </c>
       <c r="B116" s="1">
-        <v>1</v>
+        <v>1.111111111111111</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2330,7 +2270,7 @@
         <v>118</v>
       </c>
       <c r="B117" s="1">
-        <v>1.4375</v>
+        <v>1.2</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -2341,7 +2281,7 @@
         <v>119</v>
       </c>
       <c r="B118" s="1">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -2352,10 +2292,10 @@
         <v>120</v>
       </c>
       <c r="B119" s="1">
-        <v>4</v>
+        <v>1.782608695652174</v>
       </c>
       <c r="C119">
-        <v>1.888888888888889</v>
+        <v>1.454545454545455</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2363,10 +2303,10 @@
         <v>121</v>
       </c>
       <c r="B120" s="1">
-        <v>24.76666666666667</v>
+        <v>1</v>
       </c>
       <c r="C120">
-        <v>8.233333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2374,10 +2314,10 @@
         <v>122</v>
       </c>
       <c r="B121" s="1">
-        <v>1.357142857142857</v>
+        <v>1.625</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>1.176470588235294</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2388,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2396,10 +2336,10 @@
         <v>124</v>
       </c>
       <c r="B123" s="1">
-        <v>1.947368421052632</v>
+        <v>1.4</v>
       </c>
       <c r="C123">
-        <v>1.692307692307692</v>
+        <v>1.142857142857143</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2407,10 +2347,10 @@
         <v>125</v>
       </c>
       <c r="B124" s="1">
-        <v>1.166666666666667</v>
+        <v>7.866666666666666</v>
       </c>
       <c r="C124">
-        <v>1</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2418,10 +2358,10 @@
         <v>126</v>
       </c>
       <c r="B125" s="1">
-        <v>1.714285714285714</v>
+        <v>14.2</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>8.566666666666666</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2429,7 +2369,7 @@
         <v>127</v>
       </c>
       <c r="B126" s="1">
-        <v>1.166666666666667</v>
+        <v>1.2</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -2440,10 +2380,10 @@
         <v>128</v>
       </c>
       <c r="B127" s="1">
-        <v>1.2</v>
+        <v>1.739130434782609</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>1.454545454545455</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2454,7 +2394,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="C128">
-        <v>1.2</v>
+        <v>1.833333333333333</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2462,10 +2402,10 @@
         <v>130</v>
       </c>
       <c r="B129" s="1">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1.166666666666667</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2473,10 +2413,10 @@
         <v>131</v>
       </c>
       <c r="B130" s="1">
-        <v>8.199999999999999</v>
+        <v>4.428571428571429</v>
       </c>
       <c r="C130">
-        <v>2</v>
+        <v>2.363636363636364</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2487,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2495,10 +2435,10 @@
         <v>133</v>
       </c>
       <c r="B132" s="1">
-        <v>1</v>
+        <v>1.230769230769231</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2506,10 +2446,10 @@
         <v>134</v>
       </c>
       <c r="B133" s="1">
-        <v>1.444444444444444</v>
+        <v>9.333333333333334</v>
       </c>
       <c r="C133">
-        <v>1.2</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2517,10 +2457,10 @@
         <v>135</v>
       </c>
       <c r="B134" s="1">
-        <v>6.4</v>
+        <v>2.153846153846154</v>
       </c>
       <c r="C134">
-        <v>4.333333333333333</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2528,10 +2468,10 @@
         <v>136</v>
       </c>
       <c r="B135" s="1">
-        <v>12.36666666666667</v>
+        <v>1</v>
       </c>
       <c r="C135">
-        <v>8.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2539,10 +2479,10 @@
         <v>137</v>
       </c>
       <c r="B136" s="1">
-        <v>1.166666666666667</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>5.633333333333334</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2550,10 +2490,10 @@
         <v>138</v>
       </c>
       <c r="B137" s="1">
-        <v>1.666666666666667</v>
+        <v>2.384615384615385</v>
       </c>
       <c r="C137">
-        <v>1.2</v>
+        <v>1.588235294117647</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2561,10 +2501,10 @@
         <v>139</v>
       </c>
       <c r="B138" s="1">
-        <v>1.25</v>
+        <v>1.652173913043478</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>1.545454545454545</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2572,10 +2512,10 @@
         <v>140</v>
       </c>
       <c r="B139" s="1">
-        <v>1.2</v>
+        <v>5.033333333333333</v>
       </c>
       <c r="C139">
-        <v>1</v>
+        <v>2.333333333333333</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2583,10 +2523,10 @@
         <v>141</v>
       </c>
       <c r="B140" s="1">
-        <v>4.133333333333334</v>
+        <v>1.545454545454545</v>
       </c>
       <c r="C140">
-        <v>1.421052631578947</v>
+        <v>1.222222222222222</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2594,10 +2534,10 @@
         <v>142</v>
       </c>
       <c r="B141" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C141">
-        <v>1.842105263157895</v>
+        <v>3.448275862068965</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2605,10 +2545,10 @@
         <v>143</v>
       </c>
       <c r="B142" s="1">
-        <v>4.2</v>
+        <v>16.26666666666667</v>
       </c>
       <c r="C142">
-        <v>1.333333333333333</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2616,7 +2556,7 @@
         <v>144</v>
       </c>
       <c r="B143" s="1">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -2627,10 +2567,10 @@
         <v>145</v>
       </c>
       <c r="B144" s="1">
-        <v>25.16666666666667</v>
+        <v>12.83333333333333</v>
       </c>
       <c r="C144">
-        <v>8.566666666666666</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2638,10 +2578,10 @@
         <v>146</v>
       </c>
       <c r="B145" s="1">
-        <v>2.166666666666667</v>
+        <v>1</v>
       </c>
       <c r="C145">
-        <v>1.5625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2660,10 +2600,10 @@
         <v>148</v>
       </c>
       <c r="B147" s="1">
-        <v>19.46666666666667</v>
+        <v>3.689655172413793</v>
       </c>
       <c r="C147">
-        <v>5.5</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2671,10 +2611,10 @@
         <v>149</v>
       </c>
       <c r="B148" s="1">
-        <v>2.190476190476191</v>
+        <v>1</v>
       </c>
       <c r="C148">
-        <v>1.466666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2682,10 +2622,10 @@
         <v>150</v>
       </c>
       <c r="B149" s="1">
-        <v>1.4375</v>
+        <v>3.2</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2693,10 +2633,10 @@
         <v>151</v>
       </c>
       <c r="B150" s="1">
-        <v>9.5</v>
+        <v>37.1</v>
       </c>
       <c r="C150">
-        <v>2.148148148148148</v>
+        <v>35.6</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2704,10 +2644,10 @@
         <v>152</v>
       </c>
       <c r="B151" s="1">
-        <v>1.277777777777778</v>
+        <v>26.16666666666667</v>
       </c>
       <c r="C151">
-        <v>1.1</v>
+        <v>17.4</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2715,10 +2655,10 @@
         <v>153</v>
       </c>
       <c r="B152" s="1">
-        <v>13.8</v>
+        <v>1</v>
       </c>
       <c r="C152">
-        <v>3.642857142857143</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2726,10 +2666,10 @@
         <v>154</v>
       </c>
       <c r="B153" s="1">
-        <v>29.96666666666667</v>
+        <v>39.8</v>
       </c>
       <c r="C153">
-        <v>10.9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2737,10 +2677,10 @@
         <v>155</v>
       </c>
       <c r="B154" s="1">
-        <v>1</v>
+        <v>37.03333333333333</v>
       </c>
       <c r="C154">
-        <v>1</v>
+        <v>36.63333333333333</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2748,10 +2688,10 @@
         <v>156</v>
       </c>
       <c r="B155" s="1">
-        <v>16.93333333333333</v>
+        <v>1</v>
       </c>
       <c r="C155">
-        <v>6.433333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2759,10 +2699,10 @@
         <v>157</v>
       </c>
       <c r="B156" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>1.125</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2770,10 +2710,10 @@
         <v>158</v>
       </c>
       <c r="B157" s="1">
-        <v>1</v>
+        <v>2.12</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2781,10 +2721,10 @@
         <v>159</v>
       </c>
       <c r="B158" s="1">
-        <v>12.26666666666667</v>
+        <v>1</v>
       </c>
       <c r="C158">
-        <v>4.633333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2792,10 +2732,10 @@
         <v>160</v>
       </c>
       <c r="B159" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2803,10 +2743,10 @@
         <v>161</v>
       </c>
       <c r="B160" s="1">
-        <v>1</v>
+        <v>2.12</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2814,10 +2754,10 @@
         <v>162</v>
       </c>
       <c r="B161" s="1">
-        <v>2.722222222222222</v>
+        <v>2.56</v>
       </c>
       <c r="C161">
-        <v>1.583333333333333</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2825,10 +2765,10 @@
         <v>163</v>
       </c>
       <c r="B162" s="1">
-        <v>1</v>
+        <v>3.875</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2836,10 +2776,10 @@
         <v>164</v>
       </c>
       <c r="B163" s="1">
-        <v>56.56666666666667</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C163">
-        <v>35.23333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2847,10 +2787,10 @@
         <v>165</v>
       </c>
       <c r="B164" s="1">
-        <v>1</v>
+        <v>5.620689655172414</v>
       </c>
       <c r="C164">
-        <v>1</v>
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2858,10 +2798,10 @@
         <v>166</v>
       </c>
       <c r="B165" s="1">
-        <v>63.4</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C165">
-        <v>40.96666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2869,10 +2809,10 @@
         <v>167</v>
       </c>
       <c r="B166" s="1">
-        <v>58.53333333333333</v>
+        <v>3.571428571428572</v>
       </c>
       <c r="C166">
-        <v>37.3</v>
+        <v>1.863636363636364</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2880,10 +2820,10 @@
         <v>168</v>
       </c>
       <c r="B167" s="1">
-        <v>1</v>
+        <v>3.266666666666667</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>1.958333333333333</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2891,10 +2831,10 @@
         <v>169</v>
       </c>
       <c r="B168" s="1">
-        <v>1.357142857142857</v>
+        <v>3.04</v>
       </c>
       <c r="C168">
-        <v>1</v>
+        <v>2.083333333333333</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2902,10 +2842,10 @@
         <v>170</v>
       </c>
       <c r="B169" s="1">
-        <v>2.214285714285714</v>
+        <v>1.25</v>
       </c>
       <c r="C169">
-        <v>1.333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2913,10 +2853,10 @@
         <v>171</v>
       </c>
       <c r="B170" s="1">
-        <v>1</v>
+        <v>2.04</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>1.818181818181818</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2924,10 +2864,10 @@
         <v>172</v>
       </c>
       <c r="B171" s="1">
-        <v>1</v>
+        <v>3.111111111111111</v>
       </c>
       <c r="C171">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2935,10 +2875,10 @@
         <v>173</v>
       </c>
       <c r="B172" s="1">
-        <v>2.294117647058823</v>
+        <v>1.636363636363636</v>
       </c>
       <c r="C172">
-        <v>1.3</v>
+        <v>1.222222222222222</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2946,10 +2886,10 @@
         <v>174</v>
       </c>
       <c r="B173" s="1">
-        <v>2.777777777777778</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C173">
-        <v>1.363636363636364</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2957,10 +2897,10 @@
         <v>175</v>
       </c>
       <c r="B174" s="1">
-        <v>1</v>
+        <v>1.375</v>
       </c>
       <c r="C174">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2968,10 +2908,10 @@
         <v>176</v>
       </c>
       <c r="B175" s="1">
-        <v>2.266666666666667</v>
+        <v>2.52</v>
       </c>
       <c r="C175">
-        <v>2</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2979,10 +2919,10 @@
         <v>177</v>
       </c>
       <c r="B176" s="1">
-        <v>1</v>
+        <v>55.53333333333333</v>
       </c>
       <c r="C176">
-        <v>1</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2990,10 +2930,10 @@
         <v>178</v>
       </c>
       <c r="B177" s="1">
-        <v>1</v>
+        <v>1.0625</v>
       </c>
       <c r="C177">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3001,10 +2941,10 @@
         <v>179</v>
       </c>
       <c r="B178" s="1">
-        <v>4.833333333333333</v>
+        <v>1</v>
       </c>
       <c r="C178">
-        <v>2.434782608695652</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3012,10 +2952,10 @@
         <v>180</v>
       </c>
       <c r="B179" s="1">
-        <v>1</v>
+        <v>2.392857142857143</v>
       </c>
       <c r="C179">
-        <v>1</v>
+        <v>1.368421052631579</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3023,10 +2963,10 @@
         <v>181</v>
       </c>
       <c r="B180" s="1">
-        <v>2.692307692307693</v>
+        <v>1</v>
       </c>
       <c r="C180">
-        <v>1.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3034,10 +2974,10 @@
         <v>182</v>
       </c>
       <c r="B181" s="1">
-        <v>10.1</v>
+        <v>8.633333333333333</v>
       </c>
       <c r="C181">
-        <v>2.409090909090909</v>
+        <v>4.733333333333333</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3045,10 +2985,10 @@
         <v>183</v>
       </c>
       <c r="B182" s="1">
-        <v>2.666666666666667</v>
+        <v>2.043478260869565</v>
       </c>
       <c r="C182">
-        <v>1.5</v>
+        <v>1.875</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3056,7 +2996,7 @@
         <v>184</v>
       </c>
       <c r="B183" s="1">
-        <v>1</v>
+        <v>1.473684210526316</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -3067,10 +3007,10 @@
         <v>185</v>
       </c>
       <c r="B184" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C184">
-        <v>0</v>
+        <v>1.769230769230769</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3078,10 +3018,10 @@
         <v>186</v>
       </c>
       <c r="B185" s="1">
-        <v>2.117647058823529</v>
+        <v>1.083333333333333</v>
       </c>
       <c r="C185">
-        <v>1.3</v>
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3089,10 +3029,10 @@
         <v>187</v>
       </c>
       <c r="B186" s="1">
-        <v>2.761904761904762</v>
+        <v>1.931034482758621</v>
       </c>
       <c r="C186">
-        <v>1.8</v>
+        <v>1.708333333333333</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3100,10 +3040,10 @@
         <v>188</v>
       </c>
       <c r="B187" s="1">
-        <v>1.125</v>
+        <v>1.545454545454545</v>
       </c>
       <c r="C187">
-        <v>0</v>
+        <v>1.222222222222222</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3111,10 +3051,10 @@
         <v>189</v>
       </c>
       <c r="B188" s="1">
-        <v>1.333333333333333</v>
+        <v>1.458333333333333</v>
       </c>
       <c r="C188">
-        <v>1.2</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3122,10 +3062,10 @@
         <v>190</v>
       </c>
       <c r="B189" s="1">
-        <v>1.5</v>
+        <v>1.368421052631579</v>
       </c>
       <c r="C189">
-        <v>1</v>
+        <v>1.285714285714286</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3133,10 +3073,10 @@
         <v>191</v>
       </c>
       <c r="B190" s="1">
-        <v>1.214285714285714</v>
+        <v>2.12</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3144,10 +3084,10 @@
         <v>192</v>
       </c>
       <c r="B191" s="1">
-        <v>1</v>
+        <v>1.782608695652174</v>
       </c>
       <c r="C191">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3155,10 +3095,10 @@
         <v>193</v>
       </c>
       <c r="B192" s="1">
-        <v>1.894736842105263</v>
+        <v>1.090909090909091</v>
       </c>
       <c r="C192">
-        <v>1.692307692307692</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3166,10 +3106,10 @@
         <v>194</v>
       </c>
       <c r="B193" s="1">
-        <v>78.96666666666667</v>
+        <v>1.782608695652174</v>
       </c>
       <c r="C193">
-        <v>54.7</v>
+        <v>1.454545454545455</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3177,10 +3117,10 @@
         <v>195</v>
       </c>
       <c r="B194" s="1">
-        <v>1.3</v>
+        <v>1.565217391304348</v>
       </c>
       <c r="C194">
-        <v>1</v>
+        <v>1.545454545454545</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3188,10 +3128,10 @@
         <v>196</v>
       </c>
       <c r="B195" s="1">
-        <v>1</v>
+        <v>1.307692307692308</v>
       </c>
       <c r="C195">
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3199,10 +3139,10 @@
         <v>197</v>
       </c>
       <c r="B196" s="1">
-        <v>1</v>
+        <v>23.1</v>
       </c>
       <c r="C196">
-        <v>0</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3210,10 +3150,10 @@
         <v>198</v>
       </c>
       <c r="B197" s="1">
-        <v>9.766666666666667</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C197">
-        <v>1.48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3221,230 +3161,10 @@
         <v>199</v>
       </c>
       <c r="B198" s="1">
-        <v>3.379310344827586</v>
+        <v>1.739130434782609</v>
       </c>
       <c r="C198">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="A199" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B199" s="1">
-        <v>8.1</v>
-      </c>
-      <c r="C199">
-        <v>4.166666666666667</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
-      <c r="A200" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B200" s="1">
-        <v>2.615384615384615</v>
-      </c>
-      <c r="C200">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
-      <c r="A201" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B201" s="1">
-        <v>1.277777777777778</v>
-      </c>
-      <c r="C201">
-        <v>1.125</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3">
-      <c r="A202" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B202" s="1">
-        <v>1</v>
-      </c>
-      <c r="C202">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3">
-      <c r="A203" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B203" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="C203">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3">
-      <c r="A204" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B204" s="1">
-        <v>1.125</v>
-      </c>
-      <c r="C204">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
-      <c r="A205" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B205" s="1">
-        <v>13.9</v>
-      </c>
-      <c r="C205">
-        <v>2.115384615384615</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
-      <c r="A206" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B206" s="1">
-        <v>1.277777777777778</v>
-      </c>
-      <c r="C206">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3">
-      <c r="A207" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B207" s="1">
-        <v>1.625</v>
-      </c>
-      <c r="C207">
-        <v>1.444444444444444</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
-      <c r="A208" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B208" s="1">
-        <v>1</v>
-      </c>
-      <c r="C208">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3">
-      <c r="A209" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B209" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="C209">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3">
-      <c r="A210" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B210" s="1">
-        <v>2.235294117647059</v>
-      </c>
-      <c r="C210">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3">
-      <c r="A211" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B211" s="1">
-        <v>1.333333333333333</v>
-      </c>
-      <c r="C211">
-        <v>1.416666666666667</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3">
-      <c r="A212" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B212" s="1">
-        <v>1.571428571428571</v>
-      </c>
-      <c r="C212">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
-      <c r="A213" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B213" s="1">
-        <v>1.666666666666667</v>
-      </c>
-      <c r="C213">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
-      <c r="A214" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B214" s="1">
-        <v>1.461538461538461</v>
-      </c>
-      <c r="C214">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3">
-      <c r="A215" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B215" s="1">
-        <v>7.033333333333333</v>
-      </c>
-      <c r="C215">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3">
-      <c r="A216" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B216" s="1">
-        <v>40.33333333333334</v>
-      </c>
-      <c r="C216">
-        <v>22.03333333333333</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3">
-      <c r="A217" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B217" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="C217">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
-      <c r="A218" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B218" s="1">
-        <v>1.611111111111111</v>
-      </c>
-      <c r="C218">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed flywire connectome specific code
</commit_message>
<xml_diff>
--- a/results/example/rate.xlsx
+++ b/results/example/rate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t>P9</t>
   </si>
@@ -22,7 +22,7 @@
     <t>P9+BB_slnc</t>
   </si>
   <si>
-    <t>flyid</t>
+    <t>database_id</t>
   </si>
   <si>
     <t>BB_l</t>
@@ -31,6 +31,12 @@
     <t>BB_r</t>
   </si>
   <si>
+    <t>CIN-P9-1_l</t>
+  </si>
+  <si>
+    <t>CIN-P9-1_r</t>
+  </si>
+  <si>
     <t>DNa01_l</t>
   </si>
   <si>
@@ -67,24 +73,27 @@
     <t>MooDNg_l</t>
   </si>
   <si>
-    <t>P9-0DN1_l</t>
-  </si>
-  <si>
-    <t>P9-0DN1_r</t>
-  </si>
-  <si>
     <t>P9-cDN1_l</t>
   </si>
   <si>
     <t>P9-cDN1_r</t>
   </si>
   <si>
+    <t>P9-oDN1_l</t>
+  </si>
+  <si>
+    <t>P9-oDN1_r</t>
+  </si>
+  <si>
     <t>P9_l</t>
   </si>
   <si>
     <t>P9_r</t>
   </si>
   <si>
+    <t>neck motor neuron_r</t>
+  </si>
+  <si>
     <t>720575940604735660</t>
   </si>
   <si>
@@ -145,9 +154,6 @@
     <t>720575940611206514</t>
   </si>
   <si>
-    <t>720575940612629210</t>
-  </si>
-  <si>
     <t>720575940612766515</t>
   </si>
   <si>
@@ -214,9 +220,6 @@
     <t>720575940618156829</t>
   </si>
   <si>
-    <t>720575940618165393</t>
-  </si>
-  <si>
     <t>720575940618177977</t>
   </si>
   <si>
@@ -259,9 +262,6 @@
     <t>720575940620298772</t>
   </si>
   <si>
-    <t>720575940620714150</t>
-  </si>
-  <si>
     <t>720575940620746478</t>
   </si>
   <si>
@@ -313,9 +313,6 @@
     <t>720575940622933130</t>
   </si>
   <si>
-    <t>720575940622998627</t>
-  </si>
-  <si>
     <t>720575940623164515</t>
   </si>
   <si>
@@ -340,9 +337,6 @@
     <t>720575940624816115</t>
   </si>
   <si>
-    <t>720575940624943084</t>
-  </si>
-  <si>
     <t>720575940624967463</t>
   </si>
   <si>
@@ -388,6 +382,9 @@
     <t>720575940626773523</t>
   </si>
   <si>
+    <t>720575940626812218</t>
+  </si>
+  <si>
     <t>720575940626829852</t>
   </si>
   <si>
@@ -466,15 +463,15 @@
     <t>720575940630291767</t>
   </si>
   <si>
+    <t>720575940630808591</t>
+  </si>
+  <si>
     <t>720575940630931999</t>
   </si>
   <si>
     <t>720575940631283512</t>
   </si>
   <si>
-    <t>720575940631715896</t>
-  </si>
-  <si>
     <t>720575940631721785</t>
   </si>
   <si>
@@ -523,6 +520,9 @@
     <t>720575940634274017</t>
   </si>
   <si>
+    <t>720575940634295191</t>
+  </si>
+  <si>
     <t>720575940634428058</t>
   </si>
   <si>
@@ -544,6 +544,9 @@
     <t>720575940636879534</t>
   </si>
   <si>
+    <t>720575940636933751</t>
+  </si>
+  <si>
     <t>720575940637308605</t>
   </si>
   <si>
@@ -553,7 +556,7 @@
     <t>720575940638169917</t>
   </si>
   <si>
-    <t>720575940638664355</t>
+    <t>720575940638196038</t>
   </si>
   <si>
     <t>720575940638989894</t>
@@ -975,7 +978,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1008,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>109.7666666666667</v>
+        <v>109.1666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1019,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>111</v>
+        <v>111.0666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1027,10 +1030,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>28.16666666666667</v>
+        <v>2.6</v>
       </c>
       <c r="C4">
-        <v>16.33333333333333</v>
+        <v>3.033333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1038,10 +1041,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>19</v>
+        <v>6.266666666666667</v>
       </c>
       <c r="C5">
-        <v>12.2</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1049,10 +1052,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>27.43333333333333</v>
+        <v>26.93333333333333</v>
       </c>
       <c r="C6">
-        <v>15.4</v>
+        <v>16.46666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1060,10 +1063,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>10.53333333333333</v>
+        <v>18.56666666666667</v>
       </c>
       <c r="C7">
-        <v>5.8</v>
+        <v>11.86666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1071,10 +1074,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>29</v>
+        <v>26.1</v>
       </c>
       <c r="C8">
-        <v>18.6</v>
+        <v>15.53333333333333</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1082,10 +1085,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>22.83333333333333</v>
+        <v>10.96666666666667</v>
       </c>
       <c r="C9">
-        <v>12.4</v>
+        <v>5.466666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1093,10 +1096,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>11</v>
+        <v>28.13333333333333</v>
       </c>
       <c r="C10">
-        <v>6.133333333333334</v>
+        <v>17.93333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1104,10 +1107,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>8.233333333333333</v>
+        <v>23.03333333333333</v>
       </c>
       <c r="C11">
-        <v>4.466666666666667</v>
+        <v>10.96666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1115,10 +1118,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>10.4</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>6.233333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1126,10 +1129,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>1.333333333333333</v>
+        <v>8.6</v>
       </c>
       <c r="C13">
-        <v>1.421052631578947</v>
+        <v>4.233333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1137,10 +1140,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1148,10 +1151,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>5.6</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="C15">
-        <v>2.133333333333333</v>
+        <v>1.133333333333333</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1159,10 +1162,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>20.73333333333333</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C16">
-        <v>9.800000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1170,10 +1173,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="1">
-        <v>25.9</v>
+        <v>4.966666666666667</v>
       </c>
       <c r="C17">
-        <v>12.36666666666667</v>
+        <v>2.633333333333333</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1181,10 +1184,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>22.4</v>
+        <v>21.86666666666667</v>
       </c>
       <c r="C18">
-        <v>10.66666666666667</v>
+        <v>10.63333333333333</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1192,10 +1195,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>13.8</v>
+        <v>14.23333333333333</v>
       </c>
       <c r="C19">
-        <v>6.5</v>
+        <v>5.233333333333333</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1203,10 +1206,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>151.9</v>
+        <v>20.83333333333333</v>
       </c>
       <c r="C20">
-        <v>149.2</v>
+        <v>9.766666666666667</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1214,10 +1217,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>147.0333333333333</v>
+        <v>25.46666666666667</v>
       </c>
       <c r="C21">
-        <v>147.6</v>
+        <v>12.43333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1225,10 +1228,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>1.5</v>
+        <v>147.2</v>
       </c>
       <c r="C22">
-        <v>1.2</v>
+        <v>150.5666666666667</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1236,10 +1239,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>146.7</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>150.8333333333333</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1247,10 +1250,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="1">
-        <v>1.25</v>
+        <v>25.36666666666667</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1258,10 +1261,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>1.375</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="C25">
-        <v>1.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1269,10 +1272,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="1">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1280,10 +1283,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="1">
-        <v>13.9</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C27">
-        <v>13.33333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1291,10 +1294,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="1">
-        <v>9.266666666666667</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="C28">
-        <v>5.066666666666666</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1302,10 +1305,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="1">
-        <v>2.12</v>
+        <v>0.1</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1313,10 +1316,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="1">
-        <v>10.36666666666667</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>9.4</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1324,10 +1327,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="1">
-        <v>1.333333333333333</v>
+        <v>8.966666666666667</v>
       </c>
       <c r="C31">
-        <v>1.333333333333333</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1335,10 +1338,10 @@
         <v>33</v>
       </c>
       <c r="B32" s="1">
-        <v>7</v>
+        <v>1.966666666666667</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1346,10 +1349,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="1">
-        <v>7.733333333333333</v>
+        <v>9.4</v>
       </c>
       <c r="C33">
-        <v>4.433333333333334</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1357,10 +1360,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="1">
-        <v>19.36666666666667</v>
+        <v>0.8</v>
       </c>
       <c r="C34">
-        <v>14.33333333333333</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1368,10 +1371,10 @@
         <v>36</v>
       </c>
       <c r="B35" s="1">
-        <v>2.105263157894737</v>
+        <v>6.733333333333333</v>
       </c>
       <c r="C35">
-        <v>1.428571428571429</v>
+        <v>3.866666666666667</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1379,10 +1382,10 @@
         <v>37</v>
       </c>
       <c r="B36" s="1">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>4.233333333333333</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1390,10 +1393,10 @@
         <v>38</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>13.86666666666667</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1401,10 +1404,10 @@
         <v>39</v>
       </c>
       <c r="B38" s="1">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1412,10 +1415,10 @@
         <v>40</v>
       </c>
       <c r="B39" s="1">
-        <v>4.966666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C39">
-        <v>4.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1423,10 +1426,10 @@
         <v>41</v>
       </c>
       <c r="B40" s="1">
-        <v>2.64</v>
+        <v>0.1</v>
       </c>
       <c r="C40">
-        <v>1.75</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1434,10 +1437,10 @@
         <v>42</v>
       </c>
       <c r="B41" s="1">
-        <v>2.44</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C41">
-        <v>1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1445,10 +1448,10 @@
         <v>43</v>
       </c>
       <c r="B42" s="1">
-        <v>2</v>
+        <v>4.4</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>4.766666666666667</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1456,10 +1459,10 @@
         <v>44</v>
       </c>
       <c r="B43" s="1">
-        <v>2.32</v>
+        <v>2.466666666666667</v>
       </c>
       <c r="C43">
-        <v>1.75</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1467,10 +1470,10 @@
         <v>45</v>
       </c>
       <c r="B44" s="1">
-        <v>1</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0.6333333333333333</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1478,10 +1481,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="1">
-        <v>4.571428571428571</v>
+        <v>2.1</v>
       </c>
       <c r="C45">
-        <v>2.684210526315789</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1489,10 +1492,10 @@
         <v>47</v>
       </c>
       <c r="B46" s="1">
-        <v>10.5</v>
+        <v>0.1</v>
       </c>
       <c r="C46">
-        <v>10.6</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1500,10 +1503,10 @@
         <v>48</v>
       </c>
       <c r="B47" s="1">
-        <v>1.708333333333333</v>
+        <v>4.066666666666666</v>
       </c>
       <c r="C47">
-        <v>1.545454545454545</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1511,10 +1514,10 @@
         <v>49</v>
       </c>
       <c r="B48" s="1">
-        <v>3.689655172413793</v>
+        <v>10.2</v>
       </c>
       <c r="C48">
-        <v>4.466666666666667</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1522,10 +1525,10 @@
         <v>50</v>
       </c>
       <c r="B49" s="1">
-        <v>1.608695652173913</v>
+        <v>1.6</v>
       </c>
       <c r="C49">
-        <v>1.428571428571429</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1533,10 +1536,10 @@
         <v>51</v>
       </c>
       <c r="B50" s="1">
-        <v>1.25</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>4.733333333333333</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1544,10 +1547,10 @@
         <v>52</v>
       </c>
       <c r="B51" s="1">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="C51">
-        <v>1.222222222222222</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1555,10 +1558,10 @@
         <v>53</v>
       </c>
       <c r="B52" s="1">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1566,10 +1569,10 @@
         <v>54</v>
       </c>
       <c r="B53" s="1">
-        <v>2.269230769230769</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="C53">
-        <v>1.5625</v>
+        <v>0.3666666666666666</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1577,10 +1580,10 @@
         <v>55</v>
       </c>
       <c r="B54" s="1">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C54">
-        <v>1.25</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1588,10 +1591,10 @@
         <v>56</v>
       </c>
       <c r="B55" s="1">
-        <v>1.333333333333333</v>
+        <v>1.966666666666667</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1599,10 +1602,10 @@
         <v>57</v>
       </c>
       <c r="B56" s="1">
-        <v>1.739130434782609</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C56">
-        <v>1.5</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1610,10 +1613,10 @@
         <v>58</v>
       </c>
       <c r="B57" s="1">
-        <v>1.583333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C57">
-        <v>1.545454545454545</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1621,10 +1624,10 @@
         <v>59</v>
       </c>
       <c r="B58" s="1">
-        <v>28.56666666666667</v>
+        <v>1.266666666666667</v>
       </c>
       <c r="C58">
-        <v>31.63333333333333</v>
+        <v>0.3666666666666666</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1632,10 +1635,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="1">
-        <v>1.4</v>
+        <v>1.466666666666667</v>
       </c>
       <c r="C59">
-        <v>1.142857142857143</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1643,10 +1646,10 @@
         <v>61</v>
       </c>
       <c r="B60" s="1">
-        <v>2.076923076923077</v>
+        <v>27.36666666666667</v>
       </c>
       <c r="C60">
-        <v>1.470588235294118</v>
+        <v>32.46666666666667</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1654,10 +1657,10 @@
         <v>62</v>
       </c>
       <c r="B61" s="1">
-        <v>1.25</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1665,10 +1668,10 @@
         <v>63</v>
       </c>
       <c r="B62" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0.5666666666666667</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1676,10 +1679,10 @@
         <v>64</v>
       </c>
       <c r="B63" s="1">
-        <v>1</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1687,10 +1690,10 @@
         <v>65</v>
       </c>
       <c r="B64" s="1">
-        <v>4.620689655172414</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C64">
-        <v>2.103448275862069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1698,10 +1701,10 @@
         <v>66</v>
       </c>
       <c r="B65" s="1">
-        <v>6.2</v>
+        <v>0.2</v>
       </c>
       <c r="C65">
-        <v>6.433333333333334</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1709,10 +1712,10 @@
         <v>67</v>
       </c>
       <c r="B66" s="1">
-        <v>1.5</v>
+        <v>4.766666666666667</v>
       </c>
       <c r="C66">
-        <v>1.222222222222222</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1720,10 +1723,10 @@
         <v>68</v>
       </c>
       <c r="B67" s="1">
-        <v>8.033333333333333</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="C67">
-        <v>9.233333333333333</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1731,10 +1734,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="1">
-        <v>2.538461538461538</v>
+        <v>8.1</v>
       </c>
       <c r="C68">
-        <v>1.666666666666667</v>
+        <v>10.73333333333333</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1742,10 +1745,10 @@
         <v>70</v>
       </c>
       <c r="B69" s="1">
-        <v>1.739130434782609</v>
+        <v>2.133333333333333</v>
       </c>
       <c r="C69">
-        <v>1.454545454545455</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1753,10 +1756,10 @@
         <v>71</v>
       </c>
       <c r="B70" s="1">
-        <v>3.2</v>
+        <v>1.366666666666667</v>
       </c>
       <c r="C70">
-        <v>2.25</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1764,10 +1767,10 @@
         <v>72</v>
       </c>
       <c r="B71" s="1">
-        <v>4.928571428571429</v>
+        <v>2.633333333333333</v>
       </c>
       <c r="C71">
-        <v>3</v>
+        <v>0.5666666666666667</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1775,10 +1778,10 @@
         <v>73</v>
       </c>
       <c r="B72" s="1">
-        <v>3.714285714285714</v>
+        <v>4.3</v>
       </c>
       <c r="C72">
-        <v>1.863636363636364</v>
+        <v>1.366666666666667</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1786,10 +1789,10 @@
         <v>74</v>
       </c>
       <c r="B73" s="1">
-        <v>1.2</v>
+        <v>3.5</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>1.033333333333333</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1797,10 +1800,10 @@
         <v>75</v>
       </c>
       <c r="B74" s="1">
-        <v>50</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="C74">
-        <v>48.96666666666667</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1808,10 +1811,10 @@
         <v>76</v>
       </c>
       <c r="B75" s="1">
-        <v>1.25</v>
+        <v>49.2</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>49.33333333333334</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1819,10 +1822,10 @@
         <v>77</v>
       </c>
       <c r="B76" s="1">
-        <v>1.708333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C76">
-        <v>1.375</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1830,10 +1833,10 @@
         <v>78</v>
       </c>
       <c r="B77" s="1">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1841,10 +1844,10 @@
         <v>79</v>
       </c>
       <c r="B78" s="1">
-        <v>3.24</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C78">
-        <v>2.230769230769231</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1852,10 +1855,10 @@
         <v>80</v>
       </c>
       <c r="B79" s="1">
-        <v>1.904761904761905</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="C79">
-        <v>1.375</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1863,10 +1866,10 @@
         <v>81</v>
       </c>
       <c r="B80" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>0.4666666666666667</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1874,10 +1877,10 @@
         <v>82</v>
       </c>
       <c r="B81" s="1">
-        <v>15.9</v>
+        <v>14.93333333333333</v>
       </c>
       <c r="C81">
-        <v>7.733333333333333</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1885,10 +1888,10 @@
         <v>83</v>
       </c>
       <c r="B82" s="1">
-        <v>1.333333333333333</v>
+        <v>0.1</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1896,10 +1899,10 @@
         <v>84</v>
       </c>
       <c r="B83" s="1">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1907,10 +1910,10 @@
         <v>85</v>
       </c>
       <c r="B84" s="1">
-        <v>1.142857142857143</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1918,10 +1921,10 @@
         <v>86</v>
       </c>
       <c r="B85" s="1">
-        <v>1.333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1929,10 +1932,10 @@
         <v>87</v>
       </c>
       <c r="B86" s="1">
-        <v>2.423076923076923</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="C86">
-        <v>1.833333333333333</v>
+        <v>0.5333333333333333</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1940,10 +1943,10 @@
         <v>88</v>
       </c>
       <c r="B87" s="1">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1951,10 +1954,10 @@
         <v>89</v>
       </c>
       <c r="B88" s="1">
-        <v>4.633333333333334</v>
+        <v>3.933333333333333</v>
       </c>
       <c r="C88">
-        <v>4.066666666666666</v>
+        <v>4.533333333333333</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1962,10 +1965,10 @@
         <v>90</v>
       </c>
       <c r="B89" s="1">
-        <v>2.592592592592593</v>
+        <v>2</v>
       </c>
       <c r="C89">
-        <v>1.611111111111111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1973,10 +1976,10 @@
         <v>91</v>
       </c>
       <c r="B90" s="1">
-        <v>18.36666666666667</v>
+        <v>17.53333333333333</v>
       </c>
       <c r="C90">
-        <v>8.966666666666667</v>
+        <v>9.833333333333334</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1984,10 +1987,10 @@
         <v>92</v>
       </c>
       <c r="B91" s="1">
-        <v>1.333333333333333</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1995,10 +1998,10 @@
         <v>93</v>
       </c>
       <c r="B92" s="1">
-        <v>1.818181818181818</v>
+        <v>1.4</v>
       </c>
       <c r="C92">
-        <v>1.636363636363636</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2006,10 +2009,10 @@
         <v>94</v>
       </c>
       <c r="B93" s="1">
-        <v>26.83333333333333</v>
+        <v>25.73333333333333</v>
       </c>
       <c r="C93">
-        <v>23.1</v>
+        <v>22.6</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2017,10 +2020,10 @@
         <v>95</v>
       </c>
       <c r="B94" s="1">
-        <v>13.43333333333333</v>
+        <v>12.63333333333333</v>
       </c>
       <c r="C94">
-        <v>9.633333333333333</v>
+        <v>9.433333333333334</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2028,10 +2031,10 @@
         <v>96</v>
       </c>
       <c r="B95" s="1">
-        <v>6.133333333333334</v>
+        <v>5.566666666666666</v>
       </c>
       <c r="C95">
-        <v>2.931034482758621</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2039,10 +2042,10 @@
         <v>97</v>
       </c>
       <c r="B96" s="1">
-        <v>1.4</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="C96">
-        <v>1.142857142857143</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2050,10 +2053,10 @@
         <v>98</v>
       </c>
       <c r="B97" s="1">
-        <v>1.470588235294118</v>
+        <v>0.7</v>
       </c>
       <c r="C97">
-        <v>1.142857142857143</v>
+        <v>0.2333333333333333</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2061,10 +2064,10 @@
         <v>99</v>
       </c>
       <c r="B98" s="1">
-        <v>3.310344827586207</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C98">
-        <v>2.866666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2072,10 +2075,10 @@
         <v>100</v>
       </c>
       <c r="B99" s="1">
-        <v>1</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2083,10 +2086,10 @@
         <v>101</v>
       </c>
       <c r="B100" s="1">
-        <v>1.2</v>
+        <v>31.53333333333333</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>36.66666666666666</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2094,10 +2097,10 @@
         <v>102</v>
       </c>
       <c r="B101" s="1">
-        <v>31.66666666666667</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="C101">
-        <v>34.76666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2105,10 +2108,10 @@
         <v>103</v>
       </c>
       <c r="B102" s="1">
-        <v>1.153846153846154</v>
+        <v>12.06666666666667</v>
       </c>
       <c r="C102">
-        <v>1.142857142857143</v>
+        <v>3.866666666666667</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2116,10 +2119,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="1">
-        <v>12.58620689655172</v>
+        <v>6.1</v>
       </c>
       <c r="C103">
-        <v>6.4</v>
+        <v>5.766666666666667</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2127,10 +2130,10 @@
         <v>105</v>
       </c>
       <c r="B104" s="1">
-        <v>6.2</v>
+        <v>1.366666666666667</v>
       </c>
       <c r="C104">
-        <v>5.4</v>
+        <v>0.2333333333333333</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2138,10 +2141,10 @@
         <v>106</v>
       </c>
       <c r="B105" s="1">
-        <v>1.91304347826087</v>
+        <v>5.533333333333333</v>
       </c>
       <c r="C105">
-        <v>1.7</v>
+        <v>1.533333333333333</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2149,10 +2152,10 @@
         <v>107</v>
       </c>
       <c r="B106" s="1">
-        <v>5.607142857142857</v>
+        <v>0.1</v>
       </c>
       <c r="C106">
-        <v>3.227272727272727</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2160,10 +2163,10 @@
         <v>108</v>
       </c>
       <c r="B107" s="1">
-        <v>1.333333333333333</v>
+        <v>1.4</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2171,10 +2174,10 @@
         <v>109</v>
       </c>
       <c r="B108" s="1">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2182,10 +2185,10 @@
         <v>110</v>
       </c>
       <c r="B109" s="1">
-        <v>1.608695652173913</v>
+        <v>4</v>
       </c>
       <c r="C109">
-        <v>1.545454545454545</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2193,10 +2196,10 @@
         <v>111</v>
       </c>
       <c r="B110" s="1">
-        <v>1</v>
+        <v>10.4</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2204,10 +2207,10 @@
         <v>112</v>
       </c>
       <c r="B111" s="1">
-        <v>4.607142857142857</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="C111">
-        <v>2.7</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2215,10 +2218,10 @@
         <v>113</v>
       </c>
       <c r="B112" s="1">
-        <v>10.93333333333333</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C112">
-        <v>8.066666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2226,10 +2229,10 @@
         <v>114</v>
       </c>
       <c r="B113" s="1">
-        <v>1.117647058823529</v>
+        <v>2.433333333333333</v>
       </c>
       <c r="C113">
-        <v>1.4</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2237,10 +2240,10 @@
         <v>115</v>
       </c>
       <c r="B114" s="1">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2248,10 +2251,10 @@
         <v>116</v>
       </c>
       <c r="B115" s="1">
-        <v>2.56</v>
+        <v>0.4</v>
       </c>
       <c r="C115">
-        <v>1.8125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2259,10 +2262,10 @@
         <v>117</v>
       </c>
       <c r="B116" s="1">
-        <v>1.111111111111111</v>
+        <v>0.2</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2270,10 +2273,10 @@
         <v>118</v>
       </c>
       <c r="B117" s="1">
-        <v>1.2</v>
+        <v>1.366666666666667</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2281,10 +2284,10 @@
         <v>119</v>
       </c>
       <c r="B118" s="1">
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2292,10 +2295,10 @@
         <v>120</v>
       </c>
       <c r="B119" s="1">
-        <v>1.782608695652174</v>
+        <v>0.9</v>
       </c>
       <c r="C119">
-        <v>1.454545454545455</v>
+        <v>0.7333333333333333</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2303,10 +2306,10 @@
         <v>121</v>
       </c>
       <c r="B120" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2314,10 +2317,10 @@
         <v>122</v>
       </c>
       <c r="B121" s="1">
-        <v>1.625</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C121">
-        <v>1.176470588235294</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2325,10 +2328,10 @@
         <v>123</v>
       </c>
       <c r="B122" s="1">
-        <v>1</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2336,10 +2339,10 @@
         <v>124</v>
       </c>
       <c r="B123" s="1">
-        <v>1.4</v>
+        <v>7.833333333333333</v>
       </c>
       <c r="C123">
-        <v>1.142857142857143</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2347,10 +2350,10 @@
         <v>125</v>
       </c>
       <c r="B124" s="1">
-        <v>7.866666666666666</v>
+        <v>13.53333333333333</v>
       </c>
       <c r="C124">
-        <v>4.6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2358,10 +2361,10 @@
         <v>126</v>
       </c>
       <c r="B125" s="1">
-        <v>14.2</v>
+        <v>0.4</v>
       </c>
       <c r="C125">
-        <v>8.566666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2369,10 +2372,10 @@
         <v>127</v>
       </c>
       <c r="B126" s="1">
-        <v>1.2</v>
+        <v>1.366666666666667</v>
       </c>
       <c r="C126">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2380,10 +2383,10 @@
         <v>128</v>
       </c>
       <c r="B127" s="1">
-        <v>1.739130434782609</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="C127">
-        <v>1.454545454545455</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2391,10 +2394,10 @@
         <v>129</v>
       </c>
       <c r="B128" s="1">
-        <v>1.666666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="C128">
-        <v>1.833333333333333</v>
+        <v>0.7666666666666667</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2402,10 +2405,10 @@
         <v>130</v>
       </c>
       <c r="B129" s="1">
-        <v>2.25</v>
+        <v>4.2</v>
       </c>
       <c r="C129">
-        <v>1.166666666666667</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2413,10 +2416,10 @@
         <v>131</v>
       </c>
       <c r="B130" s="1">
-        <v>4.428571428571429</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C130">
-        <v>2.363636363636364</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2424,10 +2427,10 @@
         <v>132</v>
       </c>
       <c r="B131" s="1">
-        <v>1</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="C131">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2435,10 +2438,10 @@
         <v>133</v>
       </c>
       <c r="B132" s="1">
-        <v>1.230769230769231</v>
+        <v>9.166666666666666</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>9.166666666666666</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2446,10 +2449,10 @@
         <v>134</v>
       </c>
       <c r="B133" s="1">
-        <v>9.333333333333334</v>
+        <v>1.966666666666667</v>
       </c>
       <c r="C133">
-        <v>8.5</v>
+        <v>0.5666666666666667</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2457,10 +2460,10 @@
         <v>135</v>
       </c>
       <c r="B134" s="1">
-        <v>2.153846153846154</v>
+        <v>0.2</v>
       </c>
       <c r="C134">
-        <v>1.5</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2468,10 +2471,10 @@
         <v>136</v>
       </c>
       <c r="B135" s="1">
-        <v>1</v>
+        <v>5.733333333333333</v>
       </c>
       <c r="C135">
-        <v>1</v>
+        <v>6.233333333333333</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2479,10 +2482,10 @@
         <v>137</v>
       </c>
       <c r="B136" s="1">
-        <v>5.666666666666667</v>
+        <v>2.233333333333333</v>
       </c>
       <c r="C136">
-        <v>5.633333333333334</v>
+        <v>0.6333333333333333</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2490,10 +2493,10 @@
         <v>138</v>
       </c>
       <c r="B137" s="1">
-        <v>2.384615384615385</v>
+        <v>1.433333333333333</v>
       </c>
       <c r="C137">
-        <v>1.588235294117647</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2501,10 +2504,10 @@
         <v>139</v>
       </c>
       <c r="B138" s="1">
-        <v>1.652173913043478</v>
+        <v>5.266666666666667</v>
       </c>
       <c r="C138">
-        <v>1.545454545454545</v>
+        <v>1.866666666666667</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2512,10 +2515,10 @@
         <v>140</v>
       </c>
       <c r="B139" s="1">
-        <v>5.033333333333333</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="C139">
-        <v>2.333333333333333</v>
+        <v>0.3666666666666666</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2523,10 +2526,10 @@
         <v>141</v>
       </c>
       <c r="B140" s="1">
-        <v>1.545454545454545</v>
+        <v>3.233333333333333</v>
       </c>
       <c r="C140">
-        <v>1.222222222222222</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2534,10 +2537,10 @@
         <v>142</v>
       </c>
       <c r="B141" s="1">
-        <v>3</v>
+        <v>15.06666666666667</v>
       </c>
       <c r="C141">
-        <v>3.448275862068965</v>
+        <v>11.66666666666667</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2545,10 +2548,10 @@
         <v>143</v>
       </c>
       <c r="B142" s="1">
-        <v>16.26666666666667</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="C142">
-        <v>11.3</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2556,10 +2559,10 @@
         <v>144</v>
       </c>
       <c r="B143" s="1">
-        <v>1.2</v>
+        <v>12.4</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>6.466666666666667</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2567,10 +2570,10 @@
         <v>145</v>
       </c>
       <c r="B144" s="1">
-        <v>12.83333333333333</v>
+        <v>0.1</v>
       </c>
       <c r="C144">
-        <v>7.2</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2578,10 +2581,10 @@
         <v>146</v>
       </c>
       <c r="B145" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2589,10 +2592,10 @@
         <v>147</v>
       </c>
       <c r="B146" s="1">
-        <v>1</v>
+        <v>3.066666666666667</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>4.466666666666667</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2600,10 +2603,10 @@
         <v>148</v>
       </c>
       <c r="B147" s="1">
-        <v>3.689655172413793</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C147">
-        <v>4.333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2611,10 +2614,10 @@
         <v>149</v>
       </c>
       <c r="B148" s="1">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C148">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2622,10 +2625,10 @@
         <v>150</v>
       </c>
       <c r="B149" s="1">
-        <v>3.2</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="C149">
-        <v>2.25</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2633,10 +2636,10 @@
         <v>151</v>
       </c>
       <c r="B150" s="1">
-        <v>37.1</v>
+        <v>35.83333333333334</v>
       </c>
       <c r="C150">
-        <v>35.6</v>
+        <v>35.76666666666667</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2644,10 +2647,10 @@
         <v>152</v>
       </c>
       <c r="B151" s="1">
-        <v>26.16666666666667</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="C151">
-        <v>17.4</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2655,10 +2658,10 @@
         <v>153</v>
       </c>
       <c r="B152" s="1">
-        <v>1</v>
+        <v>40.23333333333333</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>41.1</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2666,10 +2669,10 @@
         <v>154</v>
       </c>
       <c r="B153" s="1">
-        <v>39.8</v>
+        <v>36.53333333333333</v>
       </c>
       <c r="C153">
-        <v>40</v>
+        <v>37.4</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2677,10 +2680,10 @@
         <v>155</v>
       </c>
       <c r="B154" s="1">
-        <v>37.03333333333333</v>
+        <v>0.1</v>
       </c>
       <c r="C154">
-        <v>36.63333333333333</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2688,10 +2691,10 @@
         <v>156</v>
       </c>
       <c r="B155" s="1">
-        <v>1</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="C155">
-        <v>1</v>
+        <v>0.2333333333333333</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2699,10 +2702,10 @@
         <v>157</v>
       </c>
       <c r="B156" s="1">
-        <v>1.5</v>
+        <v>1.966666666666667</v>
       </c>
       <c r="C156">
-        <v>1.125</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2710,10 +2713,10 @@
         <v>158</v>
       </c>
       <c r="B157" s="1">
-        <v>2.12</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C157">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2721,10 +2724,10 @@
         <v>159</v>
       </c>
       <c r="B158" s="1">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C158">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2732,10 +2735,10 @@
         <v>160</v>
       </c>
       <c r="B159" s="1">
-        <v>1.25</v>
+        <v>1.966666666666667</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2743,10 +2746,10 @@
         <v>161</v>
       </c>
       <c r="B160" s="1">
-        <v>2.12</v>
+        <v>2.233333333333333</v>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2754,10 +2757,10 @@
         <v>162</v>
       </c>
       <c r="B161" s="1">
-        <v>2.56</v>
+        <v>3.466666666666667</v>
       </c>
       <c r="C161">
-        <v>2</v>
+        <v>0.9333333333333333</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2765,10 +2768,10 @@
         <v>163</v>
       </c>
       <c r="B162" s="1">
-        <v>3.875</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C162">
-        <v>3.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2776,10 +2779,10 @@
         <v>164</v>
       </c>
       <c r="B163" s="1">
-        <v>1.333333333333333</v>
+        <v>5.5</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2787,10 +2790,10 @@
         <v>165</v>
       </c>
       <c r="B164" s="1">
-        <v>5.620689655172414</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C164">
-        <v>3.333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2798,7 +2801,7 @@
         <v>166</v>
       </c>
       <c r="B165" s="1">
-        <v>1.333333333333333</v>
+        <v>3.366666666666667</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -2809,10 +2812,10 @@
         <v>167</v>
       </c>
       <c r="B166" s="1">
-        <v>3.571428571428572</v>
+        <v>2.733333333333333</v>
       </c>
       <c r="C166">
-        <v>1.863636363636364</v>
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2820,10 +2823,10 @@
         <v>168</v>
       </c>
       <c r="B167" s="1">
-        <v>3.266666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C167">
-        <v>1.958333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2831,10 +2834,10 @@
         <v>169</v>
       </c>
       <c r="B168" s="1">
-        <v>3.04</v>
+        <v>2.566666666666667</v>
       </c>
       <c r="C168">
-        <v>2.083333333333333</v>
+        <v>0.5666666666666667</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2842,7 +2845,7 @@
         <v>170</v>
       </c>
       <c r="B169" s="1">
-        <v>1.25</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C169">
         <v>0</v>
@@ -2853,10 +2856,10 @@
         <v>171</v>
       </c>
       <c r="B170" s="1">
-        <v>2.04</v>
+        <v>1.933333333333333</v>
       </c>
       <c r="C170">
-        <v>1.818181818181818</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2864,10 +2867,10 @@
         <v>172</v>
       </c>
       <c r="B171" s="1">
-        <v>3.111111111111111</v>
+        <v>2.9</v>
       </c>
       <c r="C171">
-        <v>2</v>
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2875,10 +2878,10 @@
         <v>173</v>
       </c>
       <c r="B172" s="1">
-        <v>1.636363636363636</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="C172">
-        <v>1.222222222222222</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2886,10 +2889,10 @@
         <v>174</v>
       </c>
       <c r="B173" s="1">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C173">
-        <v>1</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2897,10 +2900,10 @@
         <v>175</v>
       </c>
       <c r="B174" s="1">
-        <v>1.375</v>
+        <v>0.7</v>
       </c>
       <c r="C174">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2908,10 +2911,10 @@
         <v>176</v>
       </c>
       <c r="B175" s="1">
-        <v>2.52</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C175">
-        <v>1.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2919,10 +2922,10 @@
         <v>177</v>
       </c>
       <c r="B176" s="1">
-        <v>55.53333333333333</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="C176">
-        <v>55.5</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2930,10 +2933,10 @@
         <v>178</v>
       </c>
       <c r="B177" s="1">
-        <v>1.0625</v>
+        <v>54.8</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2941,10 +2944,10 @@
         <v>179</v>
       </c>
       <c r="B178" s="1">
-        <v>1</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="C178">
-        <v>0</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2952,10 +2955,10 @@
         <v>180</v>
       </c>
       <c r="B179" s="1">
-        <v>2.392857142857143</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="C179">
-        <v>1.368421052631579</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2963,10 +2966,10 @@
         <v>181</v>
       </c>
       <c r="B180" s="1">
-        <v>1</v>
+        <v>2.1</v>
       </c>
       <c r="C180">
-        <v>1</v>
+        <v>1.433333333333333</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2974,10 +2977,10 @@
         <v>182</v>
       </c>
       <c r="B181" s="1">
-        <v>8.633333333333333</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C181">
-        <v>4.733333333333333</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2985,10 +2988,10 @@
         <v>183</v>
       </c>
       <c r="B182" s="1">
-        <v>2.043478260869565</v>
+        <v>8.633333333333333</v>
       </c>
       <c r="C182">
-        <v>1.875</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2996,10 +2999,10 @@
         <v>184</v>
       </c>
       <c r="B183" s="1">
-        <v>1.473684210526316</v>
+        <v>1.5</v>
       </c>
       <c r="C183">
-        <v>1</v>
+        <v>0.5333333333333333</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3007,10 +3010,10 @@
         <v>185</v>
       </c>
       <c r="B184" s="1">
-        <v>2.5</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="C184">
-        <v>1.769230769230769</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3018,10 +3021,10 @@
         <v>186</v>
       </c>
       <c r="B185" s="1">
-        <v>1.083333333333333</v>
+        <v>2.166666666666667</v>
       </c>
       <c r="C185">
-        <v>1.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3029,10 +3032,10 @@
         <v>187</v>
       </c>
       <c r="B186" s="1">
-        <v>1.931034482758621</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C186">
-        <v>1.708333333333333</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3040,10 +3043,10 @@
         <v>188</v>
       </c>
       <c r="B187" s="1">
-        <v>1.545454545454545</v>
+        <v>1.533333333333333</v>
       </c>
       <c r="C187">
-        <v>1.222222222222222</v>
+        <v>1.866666666666667</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3051,10 +3054,10 @@
         <v>189</v>
       </c>
       <c r="B188" s="1">
-        <v>1.458333333333333</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="C188">
-        <v>1.625</v>
+        <v>0.3666666666666666</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3062,10 +3065,10 @@
         <v>190</v>
       </c>
       <c r="B189" s="1">
-        <v>1.368421052631579</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="C189">
-        <v>1.285714285714286</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3073,10 +3076,10 @@
         <v>191</v>
       </c>
       <c r="B190" s="1">
-        <v>2.12</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="C190">
-        <v>2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3084,10 +3087,10 @@
         <v>192</v>
       </c>
       <c r="B191" s="1">
-        <v>1.782608695652174</v>
+        <v>1.966666666666667</v>
       </c>
       <c r="C191">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3095,10 +3098,10 @@
         <v>193</v>
       </c>
       <c r="B192" s="1">
-        <v>1.090909090909091</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C192">
-        <v>1</v>
+        <v>0.4333333333333333</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3106,10 +3109,10 @@
         <v>194</v>
       </c>
       <c r="B193" s="1">
-        <v>1.782608695652174</v>
+        <v>0.7</v>
       </c>
       <c r="C193">
-        <v>1.454545454545455</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3117,10 +3120,10 @@
         <v>195</v>
       </c>
       <c r="B194" s="1">
-        <v>1.565217391304348</v>
+        <v>1.366666666666667</v>
       </c>
       <c r="C194">
-        <v>1.545454545454545</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3128,10 +3131,10 @@
         <v>196</v>
       </c>
       <c r="B195" s="1">
-        <v>1.307692307692308</v>
+        <v>1.366666666666667</v>
       </c>
       <c r="C195">
-        <v>1.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3139,10 +3142,10 @@
         <v>197</v>
       </c>
       <c r="B196" s="1">
-        <v>23.1</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="C196">
-        <v>22.2</v>
+        <v>0.2333333333333333</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3150,10 +3153,10 @@
         <v>198</v>
       </c>
       <c r="B197" s="1">
-        <v>1.333333333333333</v>
+        <v>22.03333333333333</v>
       </c>
       <c r="C197">
-        <v>1</v>
+        <v>22.76666666666667</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3161,10 +3164,21 @@
         <v>199</v>
       </c>
       <c r="B198" s="1">
-        <v>1.739130434782609</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C198">
-        <v>1.5</v>
+        <v>0.03333333333333333</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B199" s="1">
+        <v>1.266666666666667</v>
+      </c>
+      <c r="C199">
+        <v>0.3666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>